<commit_message>
Relatório atualizado com dados de 16/12/2021.
</commit_message>
<xml_diff>
--- a/dados/Relatorio de Atividades.xlsx
+++ b/dados/Relatorio de Atividades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\R_STF\Relatorio_R\Git\Code-Relatorio\dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\R_STF\Relatorio_R\Git\Code-Relatorio\dados\Atualizados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D8BA45-AC2D-4CDF-BDF4-BFECDE76AFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C97E90D-4F0D-4849-8065-D782BD9EA7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,23 +24,12 @@
     <sheet name="Baixados" sheetId="9" r:id="rId9"/>
     <sheet name="Despacho" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029" iterateCount="1" calcOnSave="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="232">
   <si>
     <t>Porcentagem:</t>
   </si>
@@ -183,12 +172,12 @@
     <t>DIREITO ASSISTENCIAL</t>
   </si>
   <si>
+    <t>DIREITO À EDUCAÇÃO</t>
+  </si>
+  <si>
     <t>REGISTROS PÚBLICOS</t>
   </si>
   <si>
-    <t>DIREITO À EDUCAÇÃO</t>
-  </si>
-  <si>
     <t>ASSUNTO PARA PROCESSO ANTIGO</t>
   </si>
   <si>
@@ -460,6 +449,9 @@
   </si>
   <si>
     <t xml:space="preserve">NOVEMBRO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEZEMBRO </t>
   </si>
   <si>
     <t>1ª TURMA - SESSÃO VIRTUAL</t>
@@ -744,7 +736,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00%"/>
     <numFmt numFmtId="166" formatCode="d\/m\/yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -772,23 +764,6 @@
       <sz val="9"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -922,11 +897,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1042,22 +1016,13 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1072,11 +1037,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1084,25 +1055,15 @@
     <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2373,13 +2334,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3042,7 +3003,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="8.140625" customWidth="1"/>
@@ -3065,10 +3026,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="5">
-        <v>9629</v>
+        <v>9536</v>
       </c>
       <c r="D3" s="6">
-        <v>0.42888958175582398</v>
+        <v>0.42005109681966302</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3079,10 +3040,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="7">
-        <v>12822</v>
+        <v>13166</v>
       </c>
       <c r="D4" s="8">
-        <v>0.57111041824417597</v>
+        <v>0.57994890318033698</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3091,7 +3052,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="11">
-        <v>22451</v>
+        <v>22702</v>
       </c>
       <c r="D5" s="12">
         <v>1</v>
@@ -3112,10 +3073,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="5">
-        <v>21343</v>
+        <v>22403</v>
       </c>
       <c r="D8" s="6">
-        <v>0.296813940228351</v>
+        <v>0.295682817057558</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3126,10 +3087,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="7">
-        <v>50564</v>
+        <v>53364</v>
       </c>
       <c r="D9" s="8">
-        <v>0.70318605977165005</v>
+        <v>0.70431718294244205</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3138,7 +3099,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="11">
-        <v>71907</v>
+        <v>75767</v>
       </c>
       <c r="D10" s="12">
         <v>1</v>
@@ -3159,10 +3120,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="15">
-        <v>817</v>
+        <v>867</v>
       </c>
       <c r="D13" s="8">
-        <v>1.82065338503365E-2</v>
+        <v>1.8234972447734799E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -3173,10 +3134,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="16">
-        <v>44057</v>
+        <v>46679</v>
       </c>
       <c r="D14" s="8">
-        <v>0.98179346614966401</v>
+        <v>0.98176502755226502</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3185,7 +3146,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="11">
-        <v>44874</v>
+        <v>47546</v>
       </c>
       <c r="D15" s="12">
         <v>1</v>
@@ -3210,19 +3171,19 @@
         <v>2</v>
       </c>
       <c r="C18" s="15">
-        <v>20344</v>
+        <v>21330</v>
       </c>
       <c r="D18" s="8">
-        <v>0.66086278586278602</v>
+        <v>0.66351448035586502</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G18" s="15">
-        <v>30784</v>
+        <v>32147</v>
       </c>
       <c r="H18" s="8">
-        <v>0.40688360781411098</v>
+        <v>0.40338549182487798</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -3233,19 +3194,19 @@
         <v>3</v>
       </c>
       <c r="C19" s="16">
-        <v>10440</v>
+        <v>10817</v>
       </c>
       <c r="D19" s="8">
-        <v>0.33913721413721398</v>
+        <v>0.33648551964413498</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>8</v>
       </c>
       <c r="G19" s="16">
-        <v>44874</v>
+        <v>47546</v>
       </c>
       <c r="H19" s="8">
-        <v>0.59311639218588896</v>
+        <v>0.59661450817512196</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3254,14 +3215,14 @@
         <v>4</v>
       </c>
       <c r="C20" s="11">
-        <v>30784</v>
+        <v>32147</v>
       </c>
       <c r="D20" s="12">
         <v>1</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="11">
-        <v>75658</v>
+        <v>79693</v>
       </c>
       <c r="H20" s="12">
         <v>1</v>
@@ -3284,10 +3245,10 @@
         <v>11</v>
       </c>
       <c r="C23" s="15">
-        <v>14379</v>
+        <v>15061</v>
       </c>
       <c r="D23" s="8">
-        <v>0.15762644975992601</v>
+        <v>0.15699989575732301</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -3298,10 +3259,10 @@
         <v>12</v>
       </c>
       <c r="C24" s="16">
-        <v>76842</v>
+        <v>80868</v>
       </c>
       <c r="D24" s="8">
-        <v>0.84236258797219998</v>
+        <v>0.84298967997498198</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -3315,7 +3276,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="8">
-        <v>1.09622678739778E-5</v>
+        <v>1.04242676951944E-5</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3324,7 +3285,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="11">
-        <v>91222</v>
+        <v>95930</v>
       </c>
       <c r="D26" s="12">
         <v>1</v>
@@ -3347,10 +3308,10 @@
         <v>2</v>
       </c>
       <c r="C29" s="15">
-        <v>8176</v>
+        <v>8577</v>
       </c>
       <c r="D29" s="8">
-        <v>0.47034458954150599</v>
+        <v>0.46999835607430501</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -3361,10 +3322,10 @@
         <v>3</v>
       </c>
       <c r="C30" s="16">
-        <v>9207</v>
+        <v>9672</v>
       </c>
       <c r="D30" s="8">
-        <v>0.52965541045849396</v>
+        <v>0.53000164392569504</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3373,7 +3334,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="11">
-        <v>17383</v>
+        <v>18249</v>
       </c>
       <c r="D31" s="12">
         <v>1</v>
@@ -3394,10 +3355,10 @@
         <v>2</v>
       </c>
       <c r="C34" s="5">
-        <v>24878</v>
+        <v>26027</v>
       </c>
       <c r="D34" s="8">
-        <v>0.33761721877671802</v>
+        <v>0.33690164910554798</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3408,10 +3369,10 @@
         <v>3</v>
       </c>
       <c r="C35" s="7">
-        <v>48809</v>
+        <v>51227</v>
       </c>
       <c r="D35" s="8">
-        <v>0.66238278122328198</v>
+        <v>0.66309835089445202</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3420,7 +3381,7 @@
         <v>4</v>
       </c>
       <c r="C36" s="11">
-        <v>73687</v>
+        <v>77254</v>
       </c>
       <c r="D36" s="12">
         <v>1</v>
@@ -3441,7 +3402,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
   </cols>
@@ -3460,7 +3421,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.85546875" customWidth="1"/>
@@ -3478,707 +3439,714 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="39"/>
+      <c r="C2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="53"/>
+      <c r="D2" s="48"/>
       <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="I2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="43"/>
+      <c r="J2" s="39"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="47">
-        <v>1305</v>
-      </c>
-      <c r="D3" s="47"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="44">
+        <v>1228</v>
+      </c>
+      <c r="D3" s="44"/>
       <c r="E3" s="5">
-        <v>924</v>
+        <v>875</v>
       </c>
       <c r="F3" s="11">
-        <v>2229</v>
-      </c>
-      <c r="I3" s="44" t="s">
+        <v>2103</v>
+      </c>
+      <c r="I3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="44"/>
+      <c r="J3" s="40"/>
       <c r="K3" s="5">
-        <v>22384</v>
+        <v>22637</v>
       </c>
       <c r="L3" s="22">
-        <v>0.99701572313037301</v>
+        <v>0.99713681613954697</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="50">
-        <v>958</v>
-      </c>
-      <c r="D4" s="50"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="47">
+        <v>928</v>
+      </c>
+      <c r="D4" s="47"/>
       <c r="E4" s="7">
-        <v>710</v>
+        <v>686</v>
       </c>
       <c r="F4" s="11">
-        <v>1668</v>
-      </c>
-      <c r="I4" s="44" t="s">
+        <v>1614</v>
+      </c>
+      <c r="I4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="44"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="7">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L4" s="23">
-        <v>2.9842768696271898E-3</v>
+        <v>2.8631838604528202E-3</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="47">
-        <v>525</v>
-      </c>
-      <c r="D5" s="47"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="44">
+        <v>516</v>
+      </c>
+      <c r="D5" s="44"/>
       <c r="E5" s="5">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F5" s="11">
-        <v>818</v>
-      </c>
-      <c r="I5" s="45" t="s">
+        <v>804</v>
+      </c>
+      <c r="I5" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="45"/>
+      <c r="J5" s="42"/>
       <c r="K5" s="11">
-        <v>22451</v>
+        <v>22702</v>
       </c>
       <c r="L5" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="50">
-        <v>1200</v>
-      </c>
-      <c r="D6" s="50"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="47">
+        <v>1170</v>
+      </c>
+      <c r="D6" s="47"/>
       <c r="E6" s="7">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F6" s="11">
-        <v>1707</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="47">
-        <v>5641</v>
-      </c>
-      <c r="D7" s="47"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="44">
+        <v>5694</v>
+      </c>
+      <c r="D7" s="44"/>
       <c r="E7" s="5">
-        <v>10388</v>
+        <v>10811</v>
       </c>
       <c r="F7" s="11">
-        <v>16029</v>
+        <v>16505</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="48">
-        <v>9629</v>
-      </c>
-      <c r="D8" s="48"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="45">
+        <v>9536</v>
+      </c>
+      <c r="D8" s="45"/>
       <c r="E8" s="11">
-        <v>12822</v>
+        <v>13166</v>
       </c>
       <c r="F8" s="11">
-        <v>22451</v>
+        <v>22702</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="54" t="s">
+      <c r="B10" s="39"/>
+      <c r="C10" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="54"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="24" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="47">
-        <v>9044</v>
-      </c>
-      <c r="D11" s="47"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="44">
+        <v>9267</v>
+      </c>
+      <c r="D11" s="44"/>
       <c r="E11" s="22">
-        <v>0.402832835953855</v>
+        <v>0.40820192053563598</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="50">
-        <v>2760</v>
-      </c>
-      <c r="D12" s="50"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="47">
+        <v>2810</v>
+      </c>
+      <c r="D12" s="47"/>
       <c r="E12" s="23">
-        <v>0.122934390450314</v>
+        <v>0.123777640736499</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="47">
-        <v>2550</v>
-      </c>
-      <c r="D13" s="47"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="44">
+        <v>2613</v>
+      </c>
+      <c r="D13" s="44"/>
       <c r="E13" s="22">
-        <v>0.113580686829094</v>
+        <v>0.115099991190204</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="50">
+      <c r="B14" s="40"/>
+      <c r="C14" s="47">
         <v>2089</v>
       </c>
-      <c r="D14" s="50"/>
+      <c r="D14" s="47"/>
       <c r="E14" s="23">
-        <v>9.3047080308226796E-2</v>
+        <v>9.20183243767069E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="47">
-        <v>1791</v>
-      </c>
-      <c r="D15" s="47"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="44">
+        <v>1718</v>
+      </c>
+      <c r="D15" s="44"/>
       <c r="E15" s="22">
-        <v>7.9773729455258097E-2</v>
+        <v>7.5676151880891607E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="50">
-        <v>1181</v>
-      </c>
-      <c r="D16" s="50"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="47">
+        <v>1157</v>
+      </c>
+      <c r="D16" s="47"/>
       <c r="E16" s="23">
-        <v>5.2603447507906097E-2</v>
+        <v>5.0964672716060297E-2</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="47">
-        <v>926</v>
-      </c>
-      <c r="D17" s="47"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="44">
+        <v>942</v>
+      </c>
+      <c r="D17" s="44"/>
       <c r="E17" s="22">
-        <v>4.1245378824996702E-2</v>
+        <v>4.1494141485331697E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="50">
-        <v>625</v>
-      </c>
-      <c r="D18" s="50"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="47">
+        <v>653</v>
+      </c>
+      <c r="D18" s="47"/>
       <c r="E18" s="23">
-        <v>2.7838403634581999E-2</v>
+        <v>2.87639855519338E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="1" customFormat="1" ht="9.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="47">
-        <v>293</v>
-      </c>
-      <c r="D19" s="47"/>
-      <c r="E19" s="51">
-        <v>1.3050643623891999E-2</v>
-      </c>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="44">
+        <v>267</v>
+      </c>
+      <c r="D19" s="44"/>
+      <c r="E19" s="50">
+        <v>1.17610783190908E-2</v>
+      </c>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="44"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="44" t="s">
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="47">
-        <v>199</v>
-      </c>
-      <c r="I20" s="47"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="44">
+        <v>205</v>
+      </c>
+      <c r="I20" s="44"/>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" ht="9.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="50">
-        <v>266</v>
-      </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="52">
-        <v>1.18480245868781E-2</v>
-      </c>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="47">
+        <v>236</v>
+      </c>
+      <c r="D21" s="47"/>
+      <c r="E21" s="51">
+        <v>1.03955598625672E-2</v>
+      </c>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="44"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="52"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="51"/>
     </row>
     <row r="23" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="47">
-        <v>211</v>
-      </c>
-      <c r="D23" s="47"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="44">
+        <v>223</v>
+      </c>
+      <c r="D23" s="44"/>
       <c r="E23" s="22">
-        <v>9.3982450670348806E-3</v>
-      </c>
-      <c r="F23" s="43" t="s">
+        <v>9.8229230904766096E-3</v>
+      </c>
+      <c r="F23" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="43"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" ht="5.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="50">
-        <v>190</v>
-      </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="52">
-        <v>8.4628747049129201E-3</v>
-      </c>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="47">
+        <v>186</v>
+      </c>
+      <c r="D24" s="47"/>
+      <c r="E24" s="51">
+        <v>8.1931107391419299E-3</v>
+      </c>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="44"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="47"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" ht="2.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="44"/>
-      <c r="B26" s="44"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="52"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="51"/>
     </row>
     <row r="27" spans="1:9" s="1" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="47">
-        <v>168</v>
-      </c>
-      <c r="D27" s="47"/>
-      <c r="E27" s="51">
-        <v>7.4829628969756397E-3</v>
+      <c r="B27" s="40"/>
+      <c r="C27" s="44">
+        <v>171</v>
+      </c>
+      <c r="D27" s="44"/>
+      <c r="E27" s="50">
+        <v>7.5323760021143498E-3</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="1" customFormat="1" ht="3.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
-      <c r="B28" s="44"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="43" t="s">
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="43"/>
-      <c r="H28" s="46"/>
-      <c r="I28" s="46"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
     </row>
     <row r="29" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="50">
-        <v>115</v>
-      </c>
-      <c r="D29" s="50"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="47">
+        <v>118</v>
+      </c>
+      <c r="D29" s="47"/>
       <c r="E29" s="23">
-        <v>5.1222662687630798E-3</v>
-      </c>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
+        <v>5.1977799312835898E-3</v>
+      </c>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
     </row>
     <row r="30" spans="1:9" s="1" customFormat="1" ht="11.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="47">
-        <v>61</v>
-      </c>
-      <c r="D30" s="47"/>
-      <c r="E30" s="51">
-        <v>2.7170281947352E-3</v>
-      </c>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="44">
+        <v>64</v>
+      </c>
+      <c r="D30" s="44"/>
+      <c r="E30" s="50">
+        <v>2.8191348779843198E-3</v>
+      </c>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
     </row>
     <row r="31" spans="1:9" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="44"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="51"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="50"/>
     </row>
     <row r="32" spans="1:9" s="1" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="44" t="s">
+      <c r="A32" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="50">
-        <v>37</v>
-      </c>
-      <c r="D32" s="50"/>
-      <c r="E32" s="52">
-        <v>1.64803349516725E-3</v>
+      <c r="B32" s="40"/>
+      <c r="C32" s="47">
+        <v>44</v>
+      </c>
+      <c r="D32" s="47"/>
+      <c r="E32" s="51">
+        <v>1.93815522861422E-3</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="1" customFormat="1" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="44"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="52"/>
-      <c r="F33" s="43" t="s">
+      <c r="A33" s="40"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="G33" s="43"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
     </row>
     <row r="34" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="47">
-        <v>29</v>
-      </c>
-      <c r="D34" s="47"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="44">
+        <v>28</v>
+      </c>
+      <c r="D34" s="44"/>
       <c r="E34" s="22">
-        <v>1.2917019286445999E-3</v>
-      </c>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
+        <v>1.23337150911814E-3</v>
+      </c>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
     </row>
     <row r="35" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="44"/>
-      <c r="C35" s="50">
-        <v>27</v>
-      </c>
-      <c r="D35" s="50"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="47">
+        <v>28</v>
+      </c>
+      <c r="D35" s="47"/>
       <c r="E35" s="23">
-        <v>1.2026190370139399E-3</v>
-      </c>
-      <c r="F35" s="44" t="s">
+        <v>1.23337150911814E-3</v>
+      </c>
+      <c r="F35" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="G35" s="44"/>
-      <c r="H35" s="47">
-        <v>4539</v>
-      </c>
-      <c r="I35" s="47"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="44">
+        <v>5053</v>
+      </c>
+      <c r="I35" s="44"/>
     </row>
     <row r="36" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="44"/>
-      <c r="C36" s="47">
-        <v>23</v>
-      </c>
-      <c r="D36" s="47"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="44">
+        <v>24</v>
+      </c>
+      <c r="D36" s="44"/>
       <c r="E36" s="22">
-        <v>1.0244532537526201E-3</v>
-      </c>
-      <c r="F36" s="45" t="s">
+        <v>1.0571755792441199E-3</v>
+      </c>
+      <c r="F36" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G36" s="45"/>
-      <c r="H36" s="48">
-        <v>4539</v>
-      </c>
-      <c r="I36" s="48"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="45">
+        <v>5053</v>
+      </c>
+      <c r="I36" s="45"/>
     </row>
     <row r="37" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="44" t="s">
+      <c r="A37" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="44"/>
-      <c r="C37" s="50">
-        <v>21</v>
-      </c>
-      <c r="D37" s="50"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="47">
+        <v>22</v>
+      </c>
+      <c r="D37" s="47"/>
       <c r="E37" s="23">
-        <v>9.3537036212195496E-4</v>
+        <v>9.6907761430710903E-4</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="44"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="47">
-        <v>18</v>
-      </c>
-      <c r="D38" s="47"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="44">
+        <v>13</v>
+      </c>
+      <c r="D38" s="44"/>
       <c r="E38" s="22">
-        <v>8.0174602467596103E-4</v>
+        <v>5.7263677209056505E-4</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="B39" s="44"/>
-      <c r="C39" s="50">
-        <v>11</v>
-      </c>
-      <c r="D39" s="50"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="47">
+        <v>12</v>
+      </c>
+      <c r="D39" s="47"/>
       <c r="E39" s="23">
-        <v>4.8995590396864303E-4</v>
+        <v>5.2858778962205997E-4</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="44" t="s">
+      <c r="A40" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="44"/>
-      <c r="C40" s="47">
-        <v>8</v>
-      </c>
-      <c r="D40" s="47"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="44">
+        <v>10</v>
+      </c>
+      <c r="D40" s="44"/>
       <c r="E40" s="22">
-        <v>3.5633156652264898E-4</v>
+        <v>4.4048982468504998E-4</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="44" t="s">
+      <c r="A41" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="44"/>
-      <c r="C41" s="50">
+      <c r="B41" s="40"/>
+      <c r="C41" s="47">
         <v>3</v>
       </c>
-      <c r="D41" s="50"/>
+      <c r="D41" s="47"/>
       <c r="E41" s="23">
-        <v>1.3362433744599399E-4</v>
+        <v>1.3214694740551499E-4</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="44" t="s">
+      <c r="A42" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="44"/>
-      <c r="C42" s="47">
+      <c r="B42" s="40"/>
+      <c r="C42" s="44">
         <v>3</v>
       </c>
-      <c r="D42" s="47"/>
+      <c r="D42" s="44"/>
       <c r="E42" s="22">
-        <v>1.3362433744599399E-4</v>
+        <v>1.3214694740551499E-4</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="44" t="s">
+      <c r="A43" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="44"/>
-      <c r="C43" s="50">
+      <c r="B43" s="40"/>
+      <c r="C43" s="47">
         <v>1</v>
       </c>
-      <c r="D43" s="50"/>
+      <c r="D43" s="47"/>
       <c r="E43" s="23">
-        <v>4.4541445815331198E-5</v>
+        <v>4.4048982468504998E-5</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="56"/>
-      <c r="B44" s="56"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
       <c r="E44" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="45" t="s">
+      <c r="A45" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="48">
-        <v>22451</v>
-      </c>
-      <c r="D45" s="48"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="45">
+        <v>22702</v>
+      </c>
+      <c r="D45" s="45"/>
       <c r="E45" s="25"/>
     </row>
     <row r="46" spans="1:9" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="46"/>
-      <c r="C46" s="46"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
     </row>
     <row r="47" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="47">
-        <v>24</v>
-      </c>
-      <c r="C47" s="47"/>
+      <c r="B47" s="44">
+        <v>26</v>
+      </c>
+      <c r="C47" s="44"/>
     </row>
     <row r="48" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="48">
-        <v>24</v>
-      </c>
-      <c r="C48" s="48"/>
+      <c r="B48" s="45">
+        <v>26</v>
+      </c>
+      <c r="C48" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="103">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A19:B20"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B26"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A30:B31"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A32:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I21"/>
+    <mergeCell ref="H23:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H28:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H33:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G21"/>
+    <mergeCell ref="F23:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F28:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F33:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D26"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="C4:D4"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B48:C48"/>
@@ -4203,49 +4171,42 @@
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D26"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="C32:D33"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H33:I34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="F23:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F28:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F33:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I21"/>
-    <mergeCell ref="H23:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H28:I29"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A32:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A19:B20"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -4256,11 +4217,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:N56"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
@@ -4287,94 +4248,94 @@
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="6.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="47">
-        <v>50564</v>
+      <c r="B3" s="44">
+        <v>53364</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44"/>
-      <c r="B4" s="47"/>
-      <c r="I4" s="43" t="s">
+      <c r="A4" s="40"/>
+      <c r="B4" s="44"/>
+      <c r="I4" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="46"/>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="50">
-        <v>527</v>
-      </c>
-      <c r="I5" s="43"/>
-      <c r="J5" s="46"/>
+      <c r="B5" s="47">
+        <v>557</v>
+      </c>
+      <c r="I5" s="39"/>
+      <c r="J5" s="43"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="44"/>
-      <c r="B6" s="50"/>
-      <c r="I6" s="44" t="s">
+      <c r="A6" s="40"/>
+      <c r="B6" s="47"/>
+      <c r="I6" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="47">
-        <v>21343</v>
+      <c r="J6" s="44">
+        <v>22403</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="47">
-        <v>13480</v>
-      </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="47"/>
+      <c r="B7" s="44">
+        <v>14123</v>
+      </c>
+      <c r="I7" s="40"/>
+      <c r="J7" s="44"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="44"/>
-      <c r="B8" s="47"/>
-      <c r="I8" s="44" t="s">
+      <c r="A8" s="40"/>
+      <c r="B8" s="44"/>
+      <c r="I8" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="J8" s="50">
-        <v>50564</v>
+      <c r="J8" s="47">
+        <v>53364</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="50">
-        <v>7336</v>
-      </c>
-      <c r="I9" s="44"/>
-      <c r="J9" s="50"/>
+      <c r="B9" s="47">
+        <v>7723</v>
+      </c>
+      <c r="I9" s="40"/>
+      <c r="J9" s="47"/>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="44"/>
-      <c r="B10" s="50"/>
-      <c r="I10" s="45" t="s">
+      <c r="A10" s="40"/>
+      <c r="B10" s="47"/>
+      <c r="I10" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="48">
-        <v>71907</v>
+      <c r="J10" s="45">
+        <v>75767</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="48">
-        <v>71907</v>
-      </c>
-      <c r="I11" s="45"/>
-      <c r="J11" s="48"/>
+      <c r="B11" s="45">
+        <v>75767</v>
+      </c>
+      <c r="I11" s="42"/>
+      <c r="J11" s="45"/>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="45"/>
-      <c r="B12" s="48"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="45"/>
     </row>
     <row r="13" spans="1:10" s="1" customFormat="1" ht="4.7" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:10" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4396,13 +4357,13 @@
         <v>64</v>
       </c>
       <c r="B15" s="5">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>59</v>
       </c>
       <c r="G15" s="5">
-        <v>527</v>
+        <v>557</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4410,13 +4371,13 @@
         <v>65</v>
       </c>
       <c r="B16" s="7">
-        <v>39923</v>
+        <v>42158</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>60</v>
       </c>
       <c r="G16" s="7">
-        <v>13480</v>
+        <v>14123</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4424,13 +4385,13 @@
         <v>66</v>
       </c>
       <c r="B17" s="5">
-        <v>10544</v>
+        <v>11095</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G17" s="5">
-        <v>7336</v>
+        <v>7723</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4438,13 +4399,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="11">
-        <v>50564</v>
+        <v>53364</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>4</v>
       </c>
       <c r="G18" s="11">
-        <v>21343</v>
+        <v>22403</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4455,46 +4416,46 @@
       <c r="B20" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="54"/>
+      <c r="D20" s="46"/>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="5">
-        <v>30784</v>
-      </c>
-      <c r="C21" s="51">
-        <v>0.40688360781411098</v>
-      </c>
-      <c r="D21" s="51"/>
+        <v>32147</v>
+      </c>
+      <c r="C21" s="50">
+        <v>0.40338549182487798</v>
+      </c>
+      <c r="D21" s="50"/>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="7">
-        <v>44874</v>
-      </c>
-      <c r="C22" s="52">
-        <v>0.59311639218588896</v>
-      </c>
-      <c r="D22" s="52"/>
+        <v>47546</v>
+      </c>
+      <c r="C22" s="51">
+        <v>0.59661450817512196</v>
+      </c>
+      <c r="D22" s="51"/>
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="11">
-        <v>75658</v>
-      </c>
-      <c r="C23" s="57">
+        <v>79693</v>
+      </c>
+      <c r="C23" s="53">
         <v>1</v>
       </c>
-      <c r="D23" s="57"/>
+      <c r="D23" s="53"/>
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4504,46 +4465,46 @@
       <c r="B25" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="54"/>
+      <c r="D25" s="46"/>
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="5">
-        <v>10440</v>
-      </c>
-      <c r="C26" s="51">
-        <v>0.19157017817494501</v>
-      </c>
-      <c r="D26" s="51"/>
+        <v>10817</v>
+      </c>
+      <c r="C26" s="50">
+        <v>0.18813482677055801</v>
+      </c>
+      <c r="D26" s="50"/>
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="7">
-        <v>44057</v>
-      </c>
-      <c r="C27" s="52">
-        <v>0.80842982182505496</v>
-      </c>
-      <c r="D27" s="52"/>
+        <v>46679</v>
+      </c>
+      <c r="C27" s="51">
+        <v>0.81186517322944196</v>
+      </c>
+      <c r="D27" s="51"/>
     </row>
     <row r="28" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="11">
-        <v>54497</v>
-      </c>
-      <c r="C28" s="57">
+        <v>57496</v>
+      </c>
+      <c r="C28" s="53">
         <v>1</v>
       </c>
-      <c r="D28" s="57"/>
+      <c r="D28" s="53"/>
     </row>
     <row r="29" spans="1:7" s="1" customFormat="1" ht="6.4" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -4559,7 +4520,7 @@
         <v>64</v>
       </c>
       <c r="B31" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4567,7 +4528,7 @@
         <v>65</v>
       </c>
       <c r="B32" s="7">
-        <v>6479</v>
+        <v>6730</v>
       </c>
     </row>
     <row r="33" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4575,7 +4536,7 @@
         <v>66</v>
       </c>
       <c r="B33" s="5">
-        <v>3946</v>
+        <v>4071</v>
       </c>
     </row>
     <row r="34" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4583,7 +4544,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="11">
-        <v>10440</v>
+        <v>10817</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="1" customFormat="1" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4600,7 +4561,7 @@
         <v>64</v>
       </c>
       <c r="B37" s="5">
-        <v>69</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4608,7 +4569,7 @@
         <v>65</v>
       </c>
       <c r="B38" s="7">
-        <v>36955</v>
+        <v>39127</v>
       </c>
     </row>
     <row r="39" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4616,7 +4577,7 @@
         <v>66</v>
       </c>
       <c r="B39" s="5">
-        <v>7033</v>
+        <v>7460</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4624,7 +4585,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="11">
-        <v>44057</v>
+        <v>46679</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4648,7 +4609,7 @@
         <v>1</v>
       </c>
       <c r="N44" s="26">
-        <v>4770</v>
+        <v>4769</v>
       </c>
     </row>
     <row r="45" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4659,7 +4620,7 @@
         <v>2</v>
       </c>
       <c r="N45" s="7">
-        <v>5931</v>
+        <v>5930</v>
       </c>
     </row>
     <row r="46" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4670,7 +4631,7 @@
         <v>3</v>
       </c>
       <c r="N46" s="26">
-        <v>8951</v>
+        <v>8949</v>
       </c>
     </row>
     <row r="47" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4714,7 +4675,7 @@
         <v>7</v>
       </c>
       <c r="N50" s="26">
-        <v>4534</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="51" spans="12:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4725,7 +4686,7 @@
         <v>8</v>
       </c>
       <c r="N51" s="7">
-        <v>6132</v>
+        <v>6130</v>
       </c>
     </row>
     <row r="52" spans="12:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4736,7 +4697,7 @@
         <v>9</v>
       </c>
       <c r="N52" s="26">
-        <v>7040</v>
+        <v>7030</v>
       </c>
     </row>
     <row r="53" spans="12:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4747,7 +4708,7 @@
         <v>10</v>
       </c>
       <c r="N53" s="7">
-        <v>5495</v>
+        <v>5485</v>
       </c>
     </row>
     <row r="54" spans="12:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4758,22 +4719,28 @@
         <v>11</v>
       </c>
       <c r="N54" s="26">
-        <v>8355</v>
-      </c>
-    </row>
-    <row r="55" spans="12:14" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>7641</v>
+      </c>
+    </row>
+    <row r="55" spans="12:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L55" s="7">
+        <v>2021</v>
+      </c>
+      <c r="M55" s="7">
+        <v>12</v>
+      </c>
+      <c r="N55" s="7">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="56" spans="12:14" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="I10:I11"/>
@@ -4785,11 +4752,16 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -4800,11 +4772,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
@@ -4827,7 +4799,7 @@
         <v>59</v>
       </c>
       <c r="B3" s="5">
-        <v>527</v>
+        <v>557</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4835,7 +4807,7 @@
         <v>60</v>
       </c>
       <c r="B4" s="7">
-        <v>13480</v>
+        <v>14123</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4843,7 +4815,7 @@
         <v>61</v>
       </c>
       <c r="B5" s="5">
-        <v>7336</v>
+        <v>7723</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4851,7 +4823,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="11">
-        <v>21343</v>
+        <v>22403</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1" ht="22.35" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4871,7 +4843,7 @@
         <v>73</v>
       </c>
       <c r="C9" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4882,7 +4854,7 @@
         <v>74</v>
       </c>
       <c r="C10" s="7">
-        <v>379</v>
+        <v>398</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4893,7 +4865,7 @@
         <v>75</v>
       </c>
       <c r="C11" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4904,7 +4876,7 @@
         <v>76</v>
       </c>
       <c r="C12" s="7">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4913,7 +4885,7 @@
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="11">
-        <v>527</v>
+        <v>557</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4955,7 +4927,7 @@
         <v>79</v>
       </c>
       <c r="C18" s="5">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4966,7 +4938,7 @@
         <v>80</v>
       </c>
       <c r="C19" s="7">
-        <v>11558</v>
+        <v>12104</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4977,7 +4949,7 @@
         <v>81</v>
       </c>
       <c r="C20" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4988,7 +4960,7 @@
         <v>82</v>
       </c>
       <c r="C21" s="7">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5010,7 +4982,7 @@
         <v>84</v>
       </c>
       <c r="C23" s="7">
-        <v>1803</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5030,7 +5002,7 @@
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="11">
-        <v>13480</v>
+        <v>14123</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5061,7 +5033,7 @@
         <v>87</v>
       </c>
       <c r="C29" s="7">
-        <v>84</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5083,7 +5055,7 @@
         <v>89</v>
       </c>
       <c r="C31" s="7">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5094,7 +5066,7 @@
         <v>90</v>
       </c>
       <c r="C32" s="5">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5116,7 +5088,7 @@
         <v>92</v>
       </c>
       <c r="C34" s="5">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5160,7 +5132,7 @@
         <v>96</v>
       </c>
       <c r="C38" s="5">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5171,7 +5143,7 @@
         <v>97</v>
       </c>
       <c r="C39" s="7">
-        <v>575</v>
+        <v>593</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5182,7 +5154,7 @@
         <v>98</v>
       </c>
       <c r="C40" s="5">
-        <v>551</v>
+        <v>569</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5193,7 +5165,7 @@
         <v>99</v>
       </c>
       <c r="C41" s="7">
-        <v>5427</v>
+        <v>5726</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5204,7 +5176,7 @@
         <v>100</v>
       </c>
       <c r="C42" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5226,7 +5198,7 @@
         <v>102</v>
       </c>
       <c r="C44" s="5">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5237,7 +5209,7 @@
         <v>103</v>
       </c>
       <c r="C45" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5248,7 +5220,7 @@
         <v>104</v>
       </c>
       <c r="C46" s="5">
-        <v>77</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5259,7 +5231,7 @@
         <v>105</v>
       </c>
       <c r="C47" s="7">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5281,7 +5253,7 @@
         <v>107</v>
       </c>
       <c r="C49" s="7">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5301,7 +5273,7 @@
       </c>
       <c r="B51" s="9"/>
       <c r="C51" s="11">
-        <v>7336</v>
+        <v>7723</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="1" customFormat="1" ht="178.15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5324,7 +5296,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="26">
-        <v>4770</v>
+        <v>4769</v>
       </c>
     </row>
     <row r="55" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5335,7 +5307,7 @@
         <v>2</v>
       </c>
       <c r="G55" s="7">
-        <v>5931</v>
+        <v>5930</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5346,7 +5318,7 @@
         <v>3</v>
       </c>
       <c r="G56" s="26">
-        <v>8951</v>
+        <v>8949</v>
       </c>
     </row>
     <row r="57" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5390,7 +5362,7 @@
         <v>7</v>
       </c>
       <c r="G60" s="26">
-        <v>4534</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="61" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5401,7 +5373,7 @@
         <v>8</v>
       </c>
       <c r="G61" s="7">
-        <v>6132</v>
+        <v>6130</v>
       </c>
     </row>
     <row r="62" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5412,7 +5384,7 @@
         <v>9</v>
       </c>
       <c r="G62" s="26">
-        <v>7040</v>
+        <v>7030</v>
       </c>
     </row>
     <row r="63" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5423,7 +5395,7 @@
         <v>10</v>
       </c>
       <c r="G63" s="7">
-        <v>5495</v>
+        <v>5485</v>
       </c>
     </row>
     <row r="64" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5434,10 +5406,21 @@
         <v>11</v>
       </c>
       <c r="G64" s="26">
-        <v>8355</v>
-      </c>
-    </row>
-    <row r="65" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>7641</v>
+      </c>
+    </row>
+    <row r="65" spans="5:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E65" s="7">
+        <v>2021</v>
+      </c>
+      <c r="F65" s="7">
+        <v>12</v>
+      </c>
+      <c r="G65" s="7">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="66" spans="5:7" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -5448,18 +5431,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K143"/>
+  <dimension ref="A1:L143"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="10" width="26.28515625" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
-    <col min="12" max="12" width="4.7109375" customWidth="1"/>
+    <col min="2" max="11" width="26.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="70.349999999999994" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5485,14 +5466,14 @@
         <v>110</v>
       </c>
       <c r="B3" s="5">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="5">
-        <v>2574</v>
+        <v>2697</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="11">
-        <v>2615</v>
+        <v>2739</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5500,14 +5481,14 @@
         <v>111</v>
       </c>
       <c r="B4" s="7">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="7">
-        <v>3324</v>
+        <v>3538</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="11">
-        <v>3337</v>
+        <v>3552</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5515,16 +5496,16 @@
         <v>112</v>
       </c>
       <c r="B5" s="5">
-        <v>1544</v>
+        <v>1591</v>
       </c>
       <c r="C5" s="5">
-        <v>68800</v>
+        <v>72377</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="E5" s="11">
-        <v>70345</v>
+        <v>73969</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5532,14 +5513,14 @@
         <v>113</v>
       </c>
       <c r="B6" s="7">
-        <v>12657</v>
+        <v>13284</v>
       </c>
       <c r="C6" s="7">
-        <v>1610</v>
+        <v>1682</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="11">
-        <v>14267</v>
+        <v>14966</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5547,12 +5528,12 @@
         <v>114</v>
       </c>
       <c r="B7" s="5">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="11">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5561,11 +5542,11 @@
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="11">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5574,11 +5555,11 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5">
-        <v>431</v>
+        <v>469</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="11">
-        <v>431</v>
+        <v>469</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5586,16 +5567,16 @@
         <v>4</v>
       </c>
       <c r="B10" s="11">
-        <v>14379</v>
+        <v>15061</v>
       </c>
       <c r="C10" s="11">
-        <v>76842</v>
+        <v>80868</v>
       </c>
       <c r="D10" s="11">
         <v>1</v>
       </c>
       <c r="E10" s="11">
-        <v>91222</v>
+        <v>95930</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5612,7 +5593,7 @@
         <v>118</v>
       </c>
       <c r="B13" s="5">
-        <v>38669</v>
+        <v>40483</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5628,7 +5609,7 @@
         <v>120</v>
       </c>
       <c r="B15" s="5">
-        <v>38158</v>
+        <v>40370</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5636,7 +5617,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="11">
-        <v>76842</v>
+        <v>80868</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="1" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5653,7 +5634,7 @@
         <v>122</v>
       </c>
       <c r="B19" s="5">
-        <v>4712</v>
+        <v>4897</v>
       </c>
     </row>
     <row r="20" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5661,7 +5642,7 @@
         <v>123</v>
       </c>
       <c r="B20" s="7">
-        <v>9667</v>
+        <v>10164</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5669,7 +5650,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="11">
-        <v>14379</v>
+        <v>15061</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="1" customFormat="1" ht="12.2" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5685,32 +5666,32 @@
       <c r="A24" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B24" s="40">
-        <v>5504</v>
+      <c r="B24" s="5">
+        <v>5794</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B25" s="41">
-        <v>4163</v>
+      <c r="B25" s="7">
+        <v>4370</v>
       </c>
     </row>
     <row r="26" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B26" s="40">
-        <v>78</v>
+      <c r="B26" s="5">
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B27" s="41">
-        <v>4634</v>
+      <c r="B27" s="7">
+        <v>4814</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5718,7 +5699,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="11">
-        <v>14379</v>
+        <v>15061</v>
       </c>
     </row>
     <row r="29" spans="1:2" s="1" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5734,8 +5715,8 @@
       <c r="A31" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B31" s="39">
-        <v>3619</v>
+      <c r="B31" s="5">
+        <v>3767</v>
       </c>
     </row>
     <row r="32" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5743,10 +5724,10 @@
         <v>59</v>
       </c>
       <c r="B32" s="7">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>60</v>
       </c>
@@ -5754,30 +5735,30 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B34" s="7">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>83</v>
       </c>
       <c r="B35" s="5"/>
     </row>
-    <row r="36" spans="1:11" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B36" s="11">
-        <v>4712</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="1" customFormat="1" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4897</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="1" customFormat="1" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:12" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="28">
         <v>2</v>
       </c>
@@ -5805,9 +5786,12 @@
       <c r="J38" s="28">
         <v>11</v>
       </c>
-      <c r="K38" s="29"/>
-    </row>
-    <row r="39" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K38" s="28">
+        <v>12</v>
+      </c>
+      <c r="L38" s="29"/>
+    </row>
+    <row r="39" spans="1:12" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
         <v>131</v>
       </c>
@@ -5835,13 +5819,16 @@
       <c r="J39" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="K39" s="21" t="s">
+      <c r="K39" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="L39" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B40" s="5">
         <v>406</v>
@@ -5870,13 +5857,16 @@
       <c r="J40" s="5">
         <v>630</v>
       </c>
-      <c r="K40" s="11">
-        <v>5200</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K40" s="5">
+        <v>286</v>
+      </c>
+      <c r="L40" s="11">
+        <v>5486</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B41" s="7">
         <v>457</v>
@@ -5905,13 +5895,16 @@
       <c r="J41" s="7">
         <v>357</v>
       </c>
-      <c r="K41" s="11">
-        <v>4071</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K41" s="7">
+        <v>200</v>
+      </c>
+      <c r="L41" s="11">
+        <v>4271</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B42" s="5">
         <v>428</v>
@@ -5940,11 +5933,14 @@
       <c r="J42" s="5">
         <v>441</v>
       </c>
-      <c r="K42" s="11">
-        <v>4475</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K42" s="5">
+        <v>176</v>
+      </c>
+      <c r="L42" s="11">
+        <v>4651</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>4</v>
       </c>
@@ -5976,11 +5972,14 @@
         <v>1428</v>
       </c>
       <c r="K43" s="11">
-        <v>13746</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" s="1" customFormat="1" ht="45.4" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+        <v>662</v>
+      </c>
+      <c r="L43" s="11">
+        <v>14408</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="1" customFormat="1" ht="45.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:12" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
         <v>2</v>
       </c>
@@ -5991,158 +5990,158 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B46" s="5">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C46" s="5">
         <v>1</v>
       </c>
       <c r="D46" s="11">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B47" s="7">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C47" s="7">
         <v>60</v>
       </c>
       <c r="D47" s="11">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B48" s="5">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C48" s="5">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D48" s="11">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B49" s="7">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C49" s="7">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D49" s="11">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B50" s="5">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C50" s="5">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D50" s="11">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B51" s="7">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C51" s="7">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="D51" s="11">
-        <v>310</v>
+        <v>322</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B52" s="5">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C52" s="5">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D52" s="11">
-        <v>389</v>
+        <v>398</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B53" s="7">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="C53" s="7">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="D53" s="11">
-        <v>531</v>
+        <v>546</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B54" s="5">
-        <v>504</v>
+        <v>516</v>
       </c>
       <c r="C54" s="5">
-        <v>353</v>
+        <v>370</v>
       </c>
       <c r="D54" s="11">
-        <v>857</v>
+        <v>886</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B55" s="7">
-        <v>1298</v>
+        <v>1312</v>
       </c>
       <c r="C55" s="7">
-        <v>825</v>
+        <v>846</v>
       </c>
       <c r="D55" s="11">
-        <v>2123</v>
+        <v>2158</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B56" s="5">
-        <v>6938</v>
+        <v>7005</v>
       </c>
       <c r="C56" s="5">
-        <v>6545</v>
+        <v>6608</v>
       </c>
       <c r="D56" s="11">
-        <v>13483</v>
+        <v>13613</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6150,41 +6149,41 @@
         <v>21</v>
       </c>
       <c r="B57" s="7">
-        <v>25311</v>
+        <v>26727</v>
       </c>
       <c r="C57" s="7">
-        <v>46948</v>
+        <v>49982</v>
       </c>
       <c r="D57" s="11">
-        <v>72259</v>
+        <v>76709</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B58" s="5">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C58" s="5">
         <v>41</v>
       </c>
       <c r="D58" s="11">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B59" s="7">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C59" s="7">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="D59" s="11">
-        <v>421</v>
+        <v>433</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6192,13 +6191,13 @@
         <v>4</v>
       </c>
       <c r="B60" s="11">
-        <v>35558</v>
+        <v>37094</v>
       </c>
       <c r="C60" s="11">
-        <v>55664</v>
+        <v>58836</v>
       </c>
       <c r="D60" s="11">
-        <v>91222</v>
+        <v>95930</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -6251,20 +6250,20 @@
         <v>65</v>
       </c>
       <c r="C63" s="7">
-        <v>872</v>
+        <v>936</v>
       </c>
       <c r="D63" s="7">
-        <v>1027</v>
+        <v>1094</v>
       </c>
       <c r="E63" s="7"/>
       <c r="F63" s="7">
         <v>25</v>
       </c>
       <c r="G63" s="7">
-        <v>3132</v>
+        <v>3263</v>
       </c>
       <c r="H63" s="11">
-        <v>5056</v>
+        <v>5318</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6275,20 +6274,20 @@
         <v>66</v>
       </c>
       <c r="C64" s="5">
-        <v>569</v>
+        <v>602</v>
       </c>
       <c r="D64" s="5">
-        <v>549</v>
+        <v>573</v>
       </c>
       <c r="E64" s="5"/>
       <c r="F64" s="5">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G64" s="5">
-        <v>402</v>
+        <v>414</v>
       </c>
       <c r="H64" s="11">
-        <v>1573</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6303,10 +6302,10 @@
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
       <c r="G65" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H65" s="11">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6321,10 +6320,10 @@
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
       <c r="G66" s="5">
-        <v>418</v>
+        <v>434</v>
       </c>
       <c r="H66" s="11">
-        <v>418</v>
+        <v>434</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6357,10 +6356,10 @@
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
       <c r="G68" s="5">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="H68" s="11">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6411,16 +6410,16 @@
         <v>79</v>
       </c>
       <c r="C71" s="7">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D71" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
       <c r="H71" s="11">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="72" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6431,10 +6430,10 @@
         <v>80</v>
       </c>
       <c r="C72" s="5">
-        <v>2081</v>
+        <v>2175</v>
       </c>
       <c r="D72" s="5">
-        <v>1150</v>
+        <v>1207</v>
       </c>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
@@ -6442,7 +6441,7 @@
         <v>62</v>
       </c>
       <c r="H72" s="11">
-        <v>3293</v>
+        <v>3444</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6493,10 +6492,10 @@
         <v>84</v>
       </c>
       <c r="C75" s="7">
-        <v>539</v>
+        <v>562</v>
       </c>
       <c r="D75" s="7">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="E75" s="7">
         <v>1</v>
@@ -6506,7 +6505,7 @@
         <v>5</v>
       </c>
       <c r="H75" s="11">
-        <v>794</v>
+        <v>829</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6561,10 +6560,10 @@
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
       <c r="G78" s="5">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="H78" s="11">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6589,10 +6588,10 @@
         <v>89</v>
       </c>
       <c r="C80" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D80" s="5">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
@@ -6600,7 +6599,7 @@
         <v>8</v>
       </c>
       <c r="H80" s="11">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6615,10 +6614,10 @@
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
       <c r="G81" s="7">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H81" s="11">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6715,18 +6714,18 @@
         <v>97</v>
       </c>
       <c r="C87" s="7">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="D87" s="7">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
       <c r="G87" s="7">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H87" s="11">
-        <v>343</v>
+        <v>358</v>
       </c>
     </row>
     <row r="88" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6759,18 +6758,18 @@
         <v>99</v>
       </c>
       <c r="C89" s="7">
-        <v>1076</v>
+        <v>1135</v>
       </c>
       <c r="D89" s="7">
-        <v>1041</v>
+        <v>1081</v>
       </c>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
       <c r="G89" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H89" s="11">
-        <v>2126</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="90" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6813,7 +6812,7 @@
         <v>102</v>
       </c>
       <c r="C92" s="5">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D92" s="5">
         <v>17</v>
@@ -6822,7 +6821,7 @@
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="11">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="93" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6830,7 +6829,7 @@
         <v>61</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
@@ -6869,10 +6868,10 @@
       <c r="E95" s="7"/>
       <c r="F95" s="7"/>
       <c r="G95" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H95" s="11">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="96" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6887,10 +6886,10 @@
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
       <c r="G96" s="5">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H96" s="11">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="97" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6923,10 +6922,10 @@
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
       <c r="G98" s="5">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H98" s="11">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="99" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6969,36 +6968,36 @@
         <v>4</v>
       </c>
       <c r="C101" s="11">
-        <v>5504</v>
+        <v>5794</v>
       </c>
       <c r="D101" s="11">
-        <v>4163</v>
+        <v>4370</v>
       </c>
       <c r="E101" s="11">
         <v>1</v>
       </c>
       <c r="F101" s="11">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G101" s="11">
-        <v>4634</v>
+        <v>4814</v>
       </c>
       <c r="H101" s="11">
-        <v>14380</v>
+        <v>15062</v>
       </c>
     </row>
     <row r="102" spans="1:8" s="1" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="103" spans="1:8" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="104" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="30" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B104" s="30" t="s">
         <v>86</v>
@@ -7006,7 +7005,7 @@
     </row>
     <row r="105" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="31" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B105" s="31" t="s">
         <v>87</v>
@@ -7014,7 +7013,7 @@
     </row>
     <row r="106" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="30" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B106" s="30" t="s">
         <v>73</v>
@@ -7022,7 +7021,7 @@
     </row>
     <row r="107" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="31" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B107" s="31" t="s">
         <v>74</v>
@@ -7030,7 +7029,7 @@
     </row>
     <row r="108" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="30" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B108" s="30" t="s">
         <v>75</v>
@@ -7038,7 +7037,7 @@
     </row>
     <row r="109" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="31" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B109" s="31" t="s">
         <v>89</v>
@@ -7046,7 +7045,7 @@
     </row>
     <row r="110" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="30" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B110" s="30" t="s">
         <v>77</v>
@@ -7054,7 +7053,7 @@
     </row>
     <row r="111" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="31" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B111" s="31" t="s">
         <v>90</v>
@@ -7062,7 +7061,7 @@
     </row>
     <row r="112" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="30" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B112" s="30" t="s">
         <v>64</v>
@@ -7070,7 +7069,7 @@
     </row>
     <row r="113" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="31" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B113" s="31" t="s">
         <v>76</v>
@@ -7078,7 +7077,7 @@
     </row>
     <row r="114" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="30" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B114" s="30" t="s">
         <v>88</v>
@@ -7086,7 +7085,7 @@
     </row>
     <row r="115" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="31" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B115" s="31" t="s">
         <v>91</v>
@@ -7094,7 +7093,7 @@
     </row>
     <row r="116" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="30" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B116" s="30" t="s">
         <v>92</v>
@@ -7102,7 +7101,7 @@
     </row>
     <row r="117" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="31" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B117" s="31" t="s">
         <v>78</v>
@@ -7110,7 +7109,7 @@
     </row>
     <row r="118" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="30" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B118" s="30" t="s">
         <v>79</v>
@@ -7118,7 +7117,7 @@
     </row>
     <row r="119" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="31" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B119" s="31" t="s">
         <v>80</v>
@@ -7126,7 +7125,7 @@
     </row>
     <row r="120" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="30" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B120" s="30" t="s">
         <v>94</v>
@@ -7134,7 +7133,7 @@
     </row>
     <row r="121" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="31" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B121" s="31" t="s">
         <v>81</v>
@@ -7142,7 +7141,7 @@
     </row>
     <row r="122" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B122" s="30" t="s">
         <v>95</v>
@@ -7150,7 +7149,7 @@
     </row>
     <row r="123" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="31" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B123" s="31" t="s">
         <v>96</v>
@@ -7158,7 +7157,7 @@
     </row>
     <row r="124" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="30" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B124" s="30" t="s">
         <v>97</v>
@@ -7166,7 +7165,7 @@
     </row>
     <row r="125" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="31" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B125" s="31" t="s">
         <v>98</v>
@@ -7174,7 +7173,7 @@
     </row>
     <row r="126" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="30" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B126" s="30" t="s">
         <v>82</v>
@@ -7182,7 +7181,7 @@
     </row>
     <row r="127" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="31" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B127" s="31" t="s">
         <v>99</v>
@@ -7190,7 +7189,7 @@
     </row>
     <row r="128" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="30" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B128" s="30" t="s">
         <v>83</v>
@@ -7198,7 +7197,7 @@
     </row>
     <row r="129" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="31" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B129" s="31" t="s">
         <v>66</v>
@@ -7206,7 +7205,7 @@
     </row>
     <row r="130" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="30" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B130" s="30" t="s">
         <v>65</v>
@@ -7214,7 +7213,7 @@
     </row>
     <row r="131" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="31" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B131" s="31" t="s">
         <v>102</v>
@@ -7222,7 +7221,7 @@
     </row>
     <row r="132" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="30" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B132" s="30" t="s">
         <v>84</v>
@@ -7230,7 +7229,7 @@
     </row>
     <row r="133" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="31" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B133" s="31" t="s">
         <v>100</v>
@@ -7238,7 +7237,7 @@
     </row>
     <row r="134" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="30" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B134" s="30" t="s">
         <v>101</v>
@@ -7246,7 +7245,7 @@
     </row>
     <row r="135" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="31" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B135" s="31" t="s">
         <v>85</v>
@@ -7254,15 +7253,15 @@
     </row>
     <row r="136" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="30" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B136" s="30" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="137" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="31" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B137" s="31" t="s">
         <v>104</v>
@@ -7270,7 +7269,7 @@
     </row>
     <row r="138" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="30" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B138" s="30" t="s">
         <v>105</v>
@@ -7278,7 +7277,7 @@
     </row>
     <row r="139" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="31" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B139" s="31" t="s">
         <v>106</v>
@@ -7286,7 +7285,7 @@
     </row>
     <row r="140" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="30" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B140" s="30" t="s">
         <v>107</v>
@@ -7294,7 +7293,7 @@
     </row>
     <row r="141" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="31" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B141" s="31" t="s">
         <v>103</v>
@@ -7302,7 +7301,7 @@
     </row>
     <row r="142" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="30" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B142" s="30" t="s">
         <v>108</v>
@@ -7311,9 +7310,9 @@
     <row r="143" spans="1:2" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7323,7 +7322,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
@@ -7340,31 +7339,31 @@
     <row r="1" spans="1:9" s="1" customFormat="1" ht="34.15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -7375,7 +7374,7 @@
         <v>1303852</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D3" s="33">
         <v>44235</v>
@@ -7390,7 +7389,7 @@
         <v>112</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I3" s="26">
         <v>1</v>
@@ -7404,7 +7403,7 @@
         <v>1307860</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D4" s="35">
         <v>44328</v>
@@ -7419,7 +7418,7 @@
         <v>112</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I4" s="7">
         <v>1</v>
@@ -7433,7 +7432,7 @@
         <v>1309975</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D5" s="33">
         <v>44393</v>
@@ -7448,7 +7447,7 @@
         <v>112</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I5" s="26">
         <v>1</v>
@@ -7462,7 +7461,7 @@
         <v>1327899</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D6" s="35">
         <v>44370</v>
@@ -7477,7 +7476,7 @@
         <v>112</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I6" s="7">
         <v>1</v>
@@ -7491,7 +7490,7 @@
         <v>1332416</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D7" s="33">
         <v>44382</v>
@@ -7506,7 +7505,7 @@
         <v>112</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I7" s="26">
         <v>1</v>
@@ -7520,7 +7519,7 @@
         <v>1332495</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D8" s="35">
         <v>44382</v>
@@ -7535,7 +7534,7 @@
         <v>112</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I8" s="7">
         <v>1</v>
@@ -7549,7 +7548,7 @@
         <v>1333105</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D9" s="33">
         <v>44382</v>
@@ -7564,7 +7563,7 @@
         <v>112</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I9" s="26">
         <v>1</v>
@@ -7578,7 +7577,7 @@
         <v>1335466</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D10" s="35">
         <v>44390</v>
@@ -7593,7 +7592,7 @@
         <v>112</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I10" s="7">
         <v>1</v>
@@ -7607,7 +7606,7 @@
         <v>1335979</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D11" s="33">
         <v>44393</v>
@@ -7622,7 +7621,7 @@
         <v>112</v>
       </c>
       <c r="H11" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I11" s="26">
         <v>1</v>
@@ -7636,7 +7635,7 @@
         <v>1340930</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D12" s="35">
         <v>44484</v>
@@ -7651,7 +7650,7 @@
         <v>112</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I12" s="7">
         <v>1</v>
@@ -7665,7 +7664,7 @@
         <v>1341860</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D13" s="33">
         <v>44484</v>
@@ -7680,7 +7679,7 @@
         <v>112</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I13" s="26">
         <v>1</v>
@@ -7694,7 +7693,7 @@
         <v>613241</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D14" s="35">
         <v>44322</v>
@@ -7709,7 +7708,7 @@
         <v>112</v>
       </c>
       <c r="H14" s="31" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I14" s="7">
         <v>1</v>
@@ -7723,7 +7722,7 @@
         <v>1103878</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D15" s="33">
         <v>44504</v>
@@ -7738,7 +7737,7 @@
         <v>112</v>
       </c>
       <c r="H15" s="30" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I15" s="26">
         <v>1</v>
@@ -7752,7 +7751,7 @@
         <v>1303212</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D16" s="35">
         <v>44230</v>
@@ -7767,7 +7766,7 @@
         <v>112</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I16" s="7">
         <v>1</v>
@@ -7781,7 +7780,7 @@
         <v>1323228</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D17" s="33">
         <v>44474</v>
@@ -7796,7 +7795,7 @@
         <v>112</v>
       </c>
       <c r="H17" s="30" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I17" s="26">
         <v>1</v>
@@ -7844,23 +7843,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -7872,22 +7869,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="37"/>
       <c r="B3" s="5">
-        <v>35558</v>
+        <v>37094</v>
       </c>
       <c r="C3" s="5">
-        <v>55664</v>
+        <v>58836</v>
       </c>
       <c r="D3" s="11">
-        <v>91222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+        <v>95930</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:4" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
@@ -7899,24 +7896,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="37"/>
       <c r="B6" s="5">
-        <v>8176</v>
+        <v>8577</v>
       </c>
       <c r="C6" s="5">
-        <v>9207</v>
+        <v>9672</v>
       </c>
       <c r="D6" s="11">
-        <v>17383</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G7" s="42"/>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>2</v>
@@ -7928,22 +7923,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="37"/>
       <c r="B9" s="5">
-        <v>1161</v>
+        <v>1212</v>
       </c>
       <c r="C9" s="5">
-        <v>40314</v>
+        <v>42617</v>
       </c>
       <c r="D9" s="11">
-        <v>41475</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="46.35" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
+        <v>43829</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" ht="46.35" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:4" s="1" customFormat="1" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>2</v>
@@ -7955,19 +7950,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="37"/>
       <c r="B12" s="5">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="C12" s="5">
-        <v>4824</v>
+        <v>5036</v>
       </c>
       <c r="D12" s="11">
-        <v>5027</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>5247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -7980,11 +7975,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -7994,16 +7987,16 @@
     <row r="1" spans="1:2" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:2" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B3" s="5">
-        <v>15025</v>
+        <v>15792</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8019,11 +8012,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="4" width="15.42578125" customWidth="1"/>
@@ -8048,19 +8039,19 @@
     <row r="3" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="37"/>
       <c r="B3" s="5">
-        <v>24878</v>
+        <v>26027</v>
       </c>
       <c r="C3" s="5">
-        <v>48809</v>
+        <v>51227</v>
       </c>
       <c r="D3" s="11">
-        <v>73687</v>
+        <v>77254</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
@@ -8077,13 +8068,13 @@
         <v>56</v>
       </c>
       <c r="B6" s="5">
-        <v>1242</v>
+        <v>1272</v>
       </c>
       <c r="C6" s="5">
-        <v>34457</v>
+        <v>36248</v>
       </c>
       <c r="D6" s="11">
-        <v>35699</v>
+        <v>37520</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Relatório com dados de 17/12/2021.
</commit_message>
<xml_diff>
--- a/dados/Relatorio de Atividades.xlsx
+++ b/dados/Relatorio de Atividades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\R_STF\Relatorio_R\Git\Code-Relatorio\dados\Atualizados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\R_STF\Relatorio_R\Git\Code-Relatorio\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C97E90D-4F0D-4849-8065-D782BD9EA7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF818994-D915-4E84-871C-D1D1186F97C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="Baixados" sheetId="9" r:id="rId9"/>
     <sheet name="Despacho" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -166,10 +166,10 @@
     <t>DIREITO PENAL MILITAR</t>
   </si>
   <si>
+    <t>DIREITO ASSISTENCIAL</t>
+  </si>
+  <si>
     <t>DIREITO PROCESSUAL PENAL MILITAR</t>
-  </si>
-  <si>
-    <t>DIREITO ASSISTENCIAL</t>
   </si>
   <si>
     <t>DIREITO À EDUCAÇÃO</t>
@@ -1749,13 +1749,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3026,10 +3026,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="5">
-        <v>9536</v>
+        <v>9632</v>
       </c>
       <c r="D3" s="6">
-        <v>0.42005109681966302</v>
+        <v>0.419877942458588</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3040,10 +3040,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="7">
-        <v>13166</v>
+        <v>13308</v>
       </c>
       <c r="D4" s="8">
-        <v>0.57994890318033698</v>
+        <v>0.580122057541412</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3052,7 +3052,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="11">
-        <v>22702</v>
+        <v>22940</v>
       </c>
       <c r="D5" s="12">
         <v>1</v>
@@ -3073,10 +3073,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="5">
-        <v>22403</v>
+        <v>22554</v>
       </c>
       <c r="D8" s="6">
-        <v>0.295682817057558</v>
+        <v>0.29617470551929698</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3087,10 +3087,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="7">
-        <v>53364</v>
+        <v>53597</v>
       </c>
       <c r="D9" s="8">
-        <v>0.70431718294244205</v>
+        <v>0.70382529448070297</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3099,7 +3099,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="11">
-        <v>75767</v>
+        <v>76151</v>
       </c>
       <c r="D10" s="12">
         <v>1</v>
@@ -3120,10 +3120,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="15">
-        <v>867</v>
+        <v>871</v>
       </c>
       <c r="D13" s="8">
-        <v>1.8234972447734799E-2</v>
+        <v>1.8196252115236001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -3134,10 +3134,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="16">
-        <v>46679</v>
+        <v>46996</v>
       </c>
       <c r="D14" s="8">
-        <v>0.98176502755226502</v>
+        <v>0.98180374788476399</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3146,7 +3146,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="11">
-        <v>47546</v>
+        <v>47867</v>
       </c>
       <c r="D15" s="12">
         <v>1</v>
@@ -3171,19 +3171,19 @@
         <v>2</v>
       </c>
       <c r="C18" s="15">
-        <v>21330</v>
+        <v>21482</v>
       </c>
       <c r="D18" s="8">
-        <v>0.66351448035586502</v>
+        <v>0.66361867103271399</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G18" s="15">
-        <v>32147</v>
+        <v>32371</v>
       </c>
       <c r="H18" s="8">
-        <v>0.40338549182487798</v>
+        <v>0.40343727410952401</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -3194,19 +3194,19 @@
         <v>3</v>
       </c>
       <c r="C19" s="16">
-        <v>10817</v>
+        <v>10889</v>
       </c>
       <c r="D19" s="8">
-        <v>0.33648551964413498</v>
+        <v>0.33638132896728601</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>8</v>
       </c>
       <c r="G19" s="16">
-        <v>47546</v>
+        <v>47867</v>
       </c>
       <c r="H19" s="8">
-        <v>0.59661450817512196</v>
+        <v>0.59656272589047599</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3215,14 +3215,14 @@
         <v>4</v>
       </c>
       <c r="C20" s="11">
-        <v>32147</v>
+        <v>32371</v>
       </c>
       <c r="D20" s="12">
         <v>1</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="11">
-        <v>79693</v>
+        <v>80238</v>
       </c>
       <c r="H20" s="12">
         <v>1</v>
@@ -3248,7 +3248,7 @@
         <v>15061</v>
       </c>
       <c r="D23" s="8">
-        <v>0.15699989575732301</v>
+        <v>0.156117837299942</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -3259,10 +3259,10 @@
         <v>12</v>
       </c>
       <c r="C24" s="16">
-        <v>80868</v>
+        <v>81410</v>
       </c>
       <c r="D24" s="8">
-        <v>0.84298967997498198</v>
+        <v>0.843871796998093</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -3276,7 +3276,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="8">
-        <v>1.04242676951944E-5</v>
+        <v>1.03657019653371E-5</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3285,7 +3285,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="11">
-        <v>95930</v>
+        <v>96472</v>
       </c>
       <c r="D26" s="12">
         <v>1</v>
@@ -3308,10 +3308,10 @@
         <v>2</v>
       </c>
       <c r="C29" s="15">
-        <v>8577</v>
+        <v>8599</v>
       </c>
       <c r="D29" s="8">
-        <v>0.46999835607430501</v>
+        <v>0.46953150595173099</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -3322,10 +3322,10 @@
         <v>3</v>
       </c>
       <c r="C30" s="16">
-        <v>9672</v>
+        <v>9715</v>
       </c>
       <c r="D30" s="8">
-        <v>0.53000164392569504</v>
+        <v>0.53046849404826901</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3334,7 +3334,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="11">
-        <v>18249</v>
+        <v>18314</v>
       </c>
       <c r="D31" s="12">
         <v>1</v>
@@ -3355,10 +3355,10 @@
         <v>2</v>
       </c>
       <c r="C34" s="5">
-        <v>26027</v>
+        <v>26082</v>
       </c>
       <c r="D34" s="8">
-        <v>0.33690164910554798</v>
+        <v>0.33696803700162797</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3369,10 +3369,10 @@
         <v>3</v>
       </c>
       <c r="C35" s="7">
-        <v>51227</v>
+        <v>51320</v>
       </c>
       <c r="D35" s="8">
-        <v>0.66309835089445202</v>
+        <v>0.66303196299837197</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3381,7 +3381,7 @@
         <v>4</v>
       </c>
       <c r="C36" s="11">
-        <v>77254</v>
+        <v>77402</v>
       </c>
       <c r="D36" s="12">
         <v>1</v>
@@ -3468,24 +3468,24 @@
       </c>
       <c r="B3" s="40"/>
       <c r="C3" s="44">
-        <v>1228</v>
+        <v>1220</v>
       </c>
       <c r="D3" s="44"/>
       <c r="E3" s="5">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="F3" s="11">
-        <v>2103</v>
+        <v>2096</v>
       </c>
       <c r="I3" s="40" t="s">
         <v>23</v>
       </c>
       <c r="J3" s="40"/>
       <c r="K3" s="5">
-        <v>22637</v>
+        <v>22871</v>
       </c>
       <c r="L3" s="22">
-        <v>0.99713681613954697</v>
+        <v>0.99699215344376602</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3494,24 +3494,24 @@
       </c>
       <c r="B4" s="40"/>
       <c r="C4" s="47">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="D4" s="47"/>
       <c r="E4" s="7">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="F4" s="11">
-        <v>1614</v>
+        <v>1611</v>
       </c>
       <c r="I4" s="40" t="s">
         <v>24</v>
       </c>
       <c r="J4" s="40"/>
       <c r="K4" s="7">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L4" s="23">
-        <v>2.8631838604528202E-3</v>
+        <v>3.0078465562336501E-3</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3524,17 +3524,17 @@
       </c>
       <c r="D5" s="44"/>
       <c r="E5" s="5">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F5" s="11">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="I5" s="42" t="s">
         <v>4</v>
       </c>
       <c r="J5" s="42"/>
       <c r="K5" s="11">
-        <v>22702</v>
+        <v>22940</v>
       </c>
       <c r="L5" s="12">
         <v>1</v>
@@ -3562,14 +3562,14 @@
       </c>
       <c r="B7" s="40"/>
       <c r="C7" s="44">
-        <v>5694</v>
+        <v>5800</v>
       </c>
       <c r="D7" s="44"/>
       <c r="E7" s="5">
-        <v>10811</v>
+        <v>10952</v>
       </c>
       <c r="F7" s="11">
-        <v>16505</v>
+        <v>16752</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3578,14 +3578,14 @@
       </c>
       <c r="B8" s="42"/>
       <c r="C8" s="45">
-        <v>9536</v>
+        <v>9632</v>
       </c>
       <c r="D8" s="45"/>
       <c r="E8" s="11">
-        <v>13166</v>
+        <v>13308</v>
       </c>
       <c r="F8" s="11">
-        <v>22702</v>
+        <v>22940</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3608,11 +3608,11 @@
       </c>
       <c r="B11" s="40"/>
       <c r="C11" s="44">
-        <v>9267</v>
+        <v>9309</v>
       </c>
       <c r="D11" s="44"/>
       <c r="E11" s="22">
-        <v>0.40820192053563598</v>
+        <v>0.40579773321708801</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3621,11 +3621,11 @@
       </c>
       <c r="B12" s="40"/>
       <c r="C12" s="47">
-        <v>2810</v>
+        <v>2916</v>
       </c>
       <c r="D12" s="47"/>
       <c r="E12" s="23">
-        <v>0.123777640736499</v>
+        <v>0.127114210985179</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3634,11 +3634,11 @@
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="44">
-        <v>2613</v>
+        <v>2614</v>
       </c>
       <c r="D13" s="44"/>
       <c r="E13" s="22">
-        <v>0.115099991190204</v>
+        <v>0.113949433304272</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3647,11 +3647,11 @@
       </c>
       <c r="B14" s="40"/>
       <c r="C14" s="47">
-        <v>2089</v>
+        <v>2097</v>
       </c>
       <c r="D14" s="47"/>
       <c r="E14" s="23">
-        <v>9.20183243767069E-2</v>
+        <v>9.1412380122057602E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3660,11 +3660,11 @@
       </c>
       <c r="B15" s="40"/>
       <c r="C15" s="44">
-        <v>1718</v>
+        <v>1758</v>
       </c>
       <c r="D15" s="44"/>
       <c r="E15" s="22">
-        <v>7.5676151880891607E-2</v>
+        <v>7.6634699215344396E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3673,11 +3673,11 @@
       </c>
       <c r="B16" s="40"/>
       <c r="C16" s="47">
-        <v>1157</v>
+        <v>1172</v>
       </c>
       <c r="D16" s="47"/>
       <c r="E16" s="23">
-        <v>5.0964672716060297E-2</v>
+        <v>5.1089799476896298E-2</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3690,7 +3690,7 @@
       </c>
       <c r="D17" s="44"/>
       <c r="E17" s="22">
-        <v>4.1494141485331697E-2</v>
+        <v>4.1063644289450703E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3699,11 +3699,11 @@
       </c>
       <c r="B18" s="40"/>
       <c r="C18" s="47">
-        <v>653</v>
+        <v>666</v>
       </c>
       <c r="D18" s="47"/>
       <c r="E18" s="23">
-        <v>2.87639855519338E-2</v>
+        <v>2.9032258064516099E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="1" customFormat="1" ht="9.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -3712,11 +3712,11 @@
       </c>
       <c r="B19" s="40"/>
       <c r="C19" s="44">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D19" s="44"/>
       <c r="E19" s="50">
-        <v>1.17610783190908E-2</v>
+        <v>1.1769834350479499E-2</v>
       </c>
       <c r="F19" s="52"/>
       <c r="G19" s="52"/>
@@ -3734,7 +3734,7 @@
       </c>
       <c r="G20" s="40"/>
       <c r="H20" s="44">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I20" s="44"/>
     </row>
@@ -3748,7 +3748,7 @@
       </c>
       <c r="D21" s="47"/>
       <c r="E21" s="51">
-        <v>1.03955598625672E-2</v>
+        <v>1.0287707061900599E-2</v>
       </c>
       <c r="F21" s="40"/>
       <c r="G21" s="40"/>
@@ -3768,11 +3768,11 @@
       </c>
       <c r="B23" s="40"/>
       <c r="C23" s="44">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D23" s="44"/>
       <c r="E23" s="22">
-        <v>9.8229230904766096E-3</v>
+        <v>9.8081952920662605E-3</v>
       </c>
       <c r="F23" s="39" t="s">
         <v>53</v>
@@ -3787,11 +3787,11 @@
       </c>
       <c r="B24" s="40"/>
       <c r="C24" s="47">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D24" s="47"/>
       <c r="E24" s="51">
-        <v>8.1931107391419299E-3</v>
+        <v>8.1517000871839593E-3</v>
       </c>
       <c r="F24" s="39"/>
       <c r="G24" s="39"/>
@@ -3822,11 +3822,11 @@
       </c>
       <c r="B27" s="40"/>
       <c r="C27" s="44">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D27" s="44"/>
       <c r="E27" s="50">
-        <v>7.5323760021143498E-3</v>
+        <v>7.4978204010462098E-3</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="1" customFormat="1" ht="3.2" customHeight="1" x14ac:dyDescent="0.2">
@@ -3848,11 +3848,11 @@
       </c>
       <c r="B29" s="40"/>
       <c r="C29" s="47">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D29" s="47"/>
       <c r="E29" s="23">
-        <v>5.1977799312835898E-3</v>
+        <v>5.2310374891020098E-3</v>
       </c>
       <c r="F29" s="39"/>
       <c r="G29" s="39"/>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="D30" s="44"/>
       <c r="E30" s="50">
-        <v>2.8191348779843198E-3</v>
+        <v>2.7898866608544E-3</v>
       </c>
       <c r="F30" s="40"/>
       <c r="G30" s="40"/>
@@ -3893,7 +3893,7 @@
       </c>
       <c r="D32" s="47"/>
       <c r="E32" s="51">
-        <v>1.93815522861422E-3</v>
+        <v>1.9180470793373999E-3</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="1" customFormat="1" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3919,7 +3919,7 @@
       </c>
       <c r="D34" s="44"/>
       <c r="E34" s="22">
-        <v>1.23337150911814E-3</v>
+        <v>1.2205754141237999E-3</v>
       </c>
       <c r="F34" s="39"/>
       <c r="G34" s="39"/>
@@ -3932,18 +3932,18 @@
       </c>
       <c r="B35" s="40"/>
       <c r="C35" s="47">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D35" s="47"/>
       <c r="E35" s="23">
-        <v>1.23337150911814E-3</v>
+        <v>1.1333914559721E-3</v>
       </c>
       <c r="F35" s="40" t="s">
         <v>56</v>
       </c>
       <c r="G35" s="40"/>
       <c r="H35" s="44">
-        <v>5053</v>
+        <v>5246</v>
       </c>
       <c r="I35" s="44"/>
     </row>
@@ -3953,18 +3953,18 @@
       </c>
       <c r="B36" s="40"/>
       <c r="C36" s="44">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D36" s="44"/>
       <c r="E36" s="22">
-        <v>1.0571755792441199E-3</v>
+        <v>1.0897994768962499E-3</v>
       </c>
       <c r="F36" s="42" t="s">
         <v>4</v>
       </c>
       <c r="G36" s="42"/>
       <c r="H36" s="45">
-        <v>5053</v>
+        <v>5246</v>
       </c>
       <c r="I36" s="45"/>
     </row>
@@ -3974,35 +3974,35 @@
       </c>
       <c r="B37" s="40"/>
       <c r="C37" s="47">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D37" s="47"/>
       <c r="E37" s="23">
-        <v>9.6907761430710903E-4</v>
+        <v>1.0462074978204001E-3</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="40"/>
+      <c r="A38" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="B38" s="40"/>
       <c r="C38" s="44">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D38" s="44"/>
       <c r="E38" s="22">
-        <v>5.7263677209056505E-4</v>
+        <v>6.53879686137751E-4</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="40" t="s">
-        <v>47</v>
-      </c>
+      <c r="A39" s="40"/>
       <c r="B39" s="40"/>
       <c r="C39" s="47">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D39" s="47"/>
       <c r="E39" s="23">
-        <v>5.2858778962205997E-4</v>
+        <v>5.6669572798605098E-4</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4015,7 +4015,7 @@
       </c>
       <c r="D40" s="44"/>
       <c r="E40" s="22">
-        <v>4.4048982468504998E-4</v>
+        <v>4.3591979075850002E-4</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4028,7 +4028,7 @@
       </c>
       <c r="D41" s="47"/>
       <c r="E41" s="23">
-        <v>1.3214694740551499E-4</v>
+        <v>1.3077593722755001E-4</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="D42" s="44"/>
       <c r="E42" s="22">
-        <v>1.3214694740551499E-4</v>
+        <v>1.3077593722755001E-4</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4054,7 +4054,7 @@
       </c>
       <c r="D43" s="47"/>
       <c r="E43" s="23">
-        <v>4.4048982468504998E-5</v>
+        <v>4.3591979075849999E-5</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4072,7 +4072,7 @@
       </c>
       <c r="B45" s="42"/>
       <c r="C45" s="45">
-        <v>22702</v>
+        <v>22940</v>
       </c>
       <c r="D45" s="45"/>
       <c r="E45" s="25"/>
@@ -4089,7 +4089,7 @@
         <v>56</v>
       </c>
       <c r="B47" s="44">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C47" s="44"/>
     </row>
@@ -4098,7 +4098,7 @@
         <v>4</v>
       </c>
       <c r="B48" s="45">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C48" s="45"/>
     </row>
@@ -4252,7 +4252,7 @@
         <v>58</v>
       </c>
       <c r="B3" s="44">
-        <v>53364</v>
+        <v>53597</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
@@ -4268,7 +4268,7 @@
         <v>59</v>
       </c>
       <c r="B5" s="47">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="I5" s="39"/>
       <c r="J5" s="43"/>
@@ -4280,7 +4280,7 @@
         <v>2</v>
       </c>
       <c r="J6" s="44">
-        <v>22403</v>
+        <v>22554</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4288,7 +4288,7 @@
         <v>60</v>
       </c>
       <c r="B7" s="44">
-        <v>14123</v>
+        <v>14245</v>
       </c>
       <c r="I7" s="40"/>
       <c r="J7" s="44"/>
@@ -4300,7 +4300,7 @@
         <v>3</v>
       </c>
       <c r="J8" s="47">
-        <v>53364</v>
+        <v>53597</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4308,7 +4308,7 @@
         <v>61</v>
       </c>
       <c r="B9" s="47">
-        <v>7723</v>
+        <v>7750</v>
       </c>
       <c r="I9" s="40"/>
       <c r="J9" s="47"/>
@@ -4320,7 +4320,7 @@
         <v>4</v>
       </c>
       <c r="J10" s="45">
-        <v>75767</v>
+        <v>76151</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4328,7 +4328,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="45">
-        <v>75767</v>
+        <v>76151</v>
       </c>
       <c r="I11" s="42"/>
       <c r="J11" s="45"/>
@@ -4357,13 +4357,13 @@
         <v>64</v>
       </c>
       <c r="B15" s="5">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>59</v>
       </c>
       <c r="G15" s="5">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4371,13 +4371,13 @@
         <v>65</v>
       </c>
       <c r="B16" s="7">
-        <v>42158</v>
+        <v>42358</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>60</v>
       </c>
       <c r="G16" s="7">
-        <v>14123</v>
+        <v>14245</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4385,13 +4385,13 @@
         <v>66</v>
       </c>
       <c r="B17" s="5">
-        <v>11095</v>
+        <v>11127</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G17" s="5">
-        <v>7723</v>
+        <v>7750</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4399,13 +4399,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="11">
-        <v>53364</v>
+        <v>53597</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>4</v>
       </c>
       <c r="G18" s="11">
-        <v>22403</v>
+        <v>22554</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4426,10 +4426,10 @@
         <v>7</v>
       </c>
       <c r="B21" s="5">
-        <v>32147</v>
+        <v>32371</v>
       </c>
       <c r="C21" s="50">
-        <v>0.40338549182487798</v>
+        <v>0.40343727410952401</v>
       </c>
       <c r="D21" s="50"/>
     </row>
@@ -4438,10 +4438,10 @@
         <v>8</v>
       </c>
       <c r="B22" s="7">
-        <v>47546</v>
+        <v>47867</v>
       </c>
       <c r="C22" s="51">
-        <v>0.59661450817512196</v>
+        <v>0.59656272589047599</v>
       </c>
       <c r="D22" s="51"/>
     </row>
@@ -4450,7 +4450,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="11">
-        <v>79693</v>
+        <v>80238</v>
       </c>
       <c r="C23" s="53">
         <v>1</v>
@@ -4475,10 +4475,10 @@
         <v>7</v>
       </c>
       <c r="B26" s="5">
-        <v>10817</v>
+        <v>10889</v>
       </c>
       <c r="C26" s="50">
-        <v>0.18813482677055801</v>
+        <v>0.18811436468860701</v>
       </c>
       <c r="D26" s="50"/>
     </row>
@@ -4487,10 +4487,10 @@
         <v>8</v>
       </c>
       <c r="B27" s="7">
-        <v>46679</v>
+        <v>46996</v>
       </c>
       <c r="C27" s="51">
-        <v>0.81186517322944196</v>
+        <v>0.81188563531139302</v>
       </c>
       <c r="D27" s="51"/>
     </row>
@@ -4499,7 +4499,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="11">
-        <v>57496</v>
+        <v>57885</v>
       </c>
       <c r="C28" s="53">
         <v>1</v>
@@ -4528,7 +4528,7 @@
         <v>65</v>
       </c>
       <c r="B32" s="7">
-        <v>6730</v>
+        <v>6779</v>
       </c>
     </row>
     <row r="33" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4536,7 +4536,7 @@
         <v>66</v>
       </c>
       <c r="B33" s="5">
-        <v>4071</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="34" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4544,7 +4544,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="11">
-        <v>10817</v>
+        <v>10889</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="1" customFormat="1" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4569,7 +4569,7 @@
         <v>65</v>
       </c>
       <c r="B38" s="7">
-        <v>39127</v>
+        <v>39398</v>
       </c>
     </row>
     <row r="39" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4577,7 +4577,7 @@
         <v>66</v>
       </c>
       <c r="B39" s="5">
-        <v>7460</v>
+        <v>7506</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4585,7 +4585,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="11">
-        <v>46679</v>
+        <v>46996</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4686,7 +4686,7 @@
         <v>8</v>
       </c>
       <c r="N51" s="7">
-        <v>6130</v>
+        <v>6131</v>
       </c>
     </row>
     <row r="52" spans="12:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4719,7 +4719,7 @@
         <v>11</v>
       </c>
       <c r="N54" s="26">
-        <v>7641</v>
+        <v>7639</v>
       </c>
     </row>
     <row r="55" spans="12:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4730,7 +4730,7 @@
         <v>12</v>
       </c>
       <c r="N55" s="7">
-        <v>4601</v>
+        <v>4986</v>
       </c>
     </row>
     <row r="56" spans="12:14" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4799,7 +4799,7 @@
         <v>59</v>
       </c>
       <c r="B3" s="5">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4807,7 +4807,7 @@
         <v>60</v>
       </c>
       <c r="B4" s="7">
-        <v>14123</v>
+        <v>14245</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4815,7 +4815,7 @@
         <v>61</v>
       </c>
       <c r="B5" s="5">
-        <v>7723</v>
+        <v>7750</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4823,7 +4823,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="11">
-        <v>22403</v>
+        <v>22554</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1" ht="22.35" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4854,7 +4854,7 @@
         <v>74</v>
       </c>
       <c r="C10" s="7">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4876,7 +4876,7 @@
         <v>76</v>
       </c>
       <c r="C12" s="7">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4885,7 +4885,7 @@
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="11">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4938,7 +4938,7 @@
         <v>80</v>
       </c>
       <c r="C19" s="7">
-        <v>12104</v>
+        <v>12213</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4960,7 +4960,7 @@
         <v>82</v>
       </c>
       <c r="C21" s="7">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4982,7 +4982,7 @@
         <v>84</v>
       </c>
       <c r="C23" s="7">
-        <v>1895</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5002,7 +5002,7 @@
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="11">
-        <v>14123</v>
+        <v>14245</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5033,7 +5033,7 @@
         <v>87</v>
       </c>
       <c r="C29" s="7">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5066,7 +5066,7 @@
         <v>90</v>
       </c>
       <c r="C32" s="5">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5143,7 +5143,7 @@
         <v>97</v>
       </c>
       <c r="C39" s="7">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5154,7 +5154,7 @@
         <v>98</v>
       </c>
       <c r="C40" s="5">
-        <v>569</v>
+        <v>571</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5165,7 +5165,7 @@
         <v>99</v>
       </c>
       <c r="C41" s="7">
-        <v>5726</v>
+        <v>5746</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5253,7 +5253,7 @@
         <v>107</v>
       </c>
       <c r="C49" s="7">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5273,7 +5273,7 @@
       </c>
       <c r="B51" s="9"/>
       <c r="C51" s="11">
-        <v>7723</v>
+        <v>7750</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="1" customFormat="1" ht="178.15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5373,7 +5373,7 @@
         <v>8</v>
       </c>
       <c r="G61" s="7">
-        <v>6130</v>
+        <v>6131</v>
       </c>
     </row>
     <row r="62" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5406,7 +5406,7 @@
         <v>11</v>
       </c>
       <c r="G64" s="26">
-        <v>7641</v>
+        <v>7639</v>
       </c>
     </row>
     <row r="65" spans="5:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5417,7 +5417,7 @@
         <v>12</v>
       </c>
       <c r="G65" s="7">
-        <v>4601</v>
+        <v>4986</v>
       </c>
     </row>
     <row r="66" spans="5:7" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5469,11 +5469,11 @@
         <v>42</v>
       </c>
       <c r="C3" s="5">
-        <v>2697</v>
+        <v>2723</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="11">
-        <v>2739</v>
+        <v>2765</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5484,11 +5484,11 @@
         <v>14</v>
       </c>
       <c r="C4" s="7">
-        <v>3538</v>
+        <v>3578</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="11">
-        <v>3552</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5499,13 +5499,13 @@
         <v>1591</v>
       </c>
       <c r="C5" s="5">
-        <v>72377</v>
+        <v>72831</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="E5" s="11">
-        <v>73969</v>
+        <v>74423</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5513,14 +5513,14 @@
         <v>113</v>
       </c>
       <c r="B6" s="7">
-        <v>13284</v>
+        <v>13283</v>
       </c>
       <c r="C6" s="7">
-        <v>1682</v>
+        <v>1698</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="11">
-        <v>14966</v>
+        <v>14981</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5528,12 +5528,12 @@
         <v>114</v>
       </c>
       <c r="B7" s="5">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="11">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5555,11 +5555,11 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="11">
-        <v>469</v>
+        <v>475</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5570,13 +5570,13 @@
         <v>15061</v>
       </c>
       <c r="C10" s="11">
-        <v>80868</v>
+        <v>81410</v>
       </c>
       <c r="D10" s="11">
         <v>1</v>
       </c>
       <c r="E10" s="11">
-        <v>95930</v>
+        <v>96472</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5593,7 +5593,7 @@
         <v>118</v>
       </c>
       <c r="B13" s="5">
-        <v>40483</v>
+        <v>40811</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5609,7 +5609,7 @@
         <v>120</v>
       </c>
       <c r="B15" s="5">
-        <v>40370</v>
+        <v>40584</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5617,7 +5617,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="11">
-        <v>80868</v>
+        <v>81410</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="1" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6051,13 +6051,13 @@
         <v>148</v>
       </c>
       <c r="B50" s="5">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C50" s="5">
         <v>73</v>
       </c>
       <c r="D50" s="11">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6065,13 +6065,13 @@
         <v>149</v>
       </c>
       <c r="B51" s="7">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C51" s="7">
         <v>120</v>
       </c>
       <c r="D51" s="11">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6093,13 +6093,13 @@
         <v>151</v>
       </c>
       <c r="B53" s="7">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C53" s="7">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D53" s="11">
-        <v>546</v>
+        <v>550</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6121,13 +6121,13 @@
         <v>153</v>
       </c>
       <c r="B55" s="7">
-        <v>1312</v>
+        <v>1317</v>
       </c>
       <c r="C55" s="7">
-        <v>846</v>
+        <v>849</v>
       </c>
       <c r="D55" s="11">
-        <v>2158</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6135,13 +6135,13 @@
         <v>154</v>
       </c>
       <c r="B56" s="5">
-        <v>7005</v>
+        <v>7013</v>
       </c>
       <c r="C56" s="5">
-        <v>6608</v>
+        <v>6609</v>
       </c>
       <c r="D56" s="11">
-        <v>13613</v>
+        <v>13622</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6149,13 +6149,13 @@
         <v>21</v>
       </c>
       <c r="B57" s="7">
-        <v>26727</v>
+        <v>26979</v>
       </c>
       <c r="C57" s="7">
-        <v>49982</v>
+        <v>50248</v>
       </c>
       <c r="D57" s="11">
-        <v>76709</v>
+        <v>77227</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6191,13 +6191,13 @@
         <v>4</v>
       </c>
       <c r="B60" s="11">
-        <v>37094</v>
+        <v>37364</v>
       </c>
       <c r="C60" s="11">
-        <v>58836</v>
+        <v>59108</v>
       </c>
       <c r="D60" s="11">
-        <v>95930</v>
+        <v>96472</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -7872,13 +7872,13 @@
     <row r="3" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="37"/>
       <c r="B3" s="5">
-        <v>37094</v>
+        <v>37364</v>
       </c>
       <c r="C3" s="5">
-        <v>58836</v>
+        <v>59108</v>
       </c>
       <c r="D3" s="11">
-        <v>95930</v>
+        <v>96472</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7899,13 +7899,13 @@
     <row r="6" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="37"/>
       <c r="B6" s="5">
-        <v>8577</v>
+        <v>8599</v>
       </c>
       <c r="C6" s="5">
-        <v>9672</v>
+        <v>9715</v>
       </c>
       <c r="D6" s="11">
-        <v>18249</v>
+        <v>18314</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7926,13 +7926,13 @@
     <row r="9" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="37"/>
       <c r="B9" s="5">
-        <v>1212</v>
+        <v>1220</v>
       </c>
       <c r="C9" s="5">
-        <v>42617</v>
+        <v>42823</v>
       </c>
       <c r="D9" s="11">
-        <v>43829</v>
+        <v>44043</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" ht="46.35" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7953,13 +7953,13 @@
     <row r="12" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="37"/>
       <c r="B12" s="5">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C12" s="5">
-        <v>5036</v>
+        <v>5059</v>
       </c>
       <c r="D12" s="11">
-        <v>5247</v>
+        <v>5271</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7975,7 +7975,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7996,7 +7998,7 @@
         <v>230</v>
       </c>
       <c r="B3" s="5">
-        <v>15792</v>
+        <v>15876</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8039,13 +8041,13 @@
     <row r="3" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="37"/>
       <c r="B3" s="5">
-        <v>26027</v>
+        <v>26082</v>
       </c>
       <c r="C3" s="5">
-        <v>51227</v>
+        <v>51320</v>
       </c>
       <c r="D3" s="11">
-        <v>77254</v>
+        <v>77402</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8071,10 +8073,10 @@
         <v>1272</v>
       </c>
       <c r="C6" s="5">
-        <v>36248</v>
+        <v>36312</v>
       </c>
       <c r="D6" s="11">
-        <v>37520</v>
+        <v>37584</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Relatório atualizado com dados de 01/01/2022.
</commit_message>
<xml_diff>
--- a/dados/Relatorio de Atividades.xlsx
+++ b/dados/Relatorio de Atividades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Downloads\STF-01-01-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E757516C-2E1A-4660-985A-6A5023AD009A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF0B49D-136C-45F9-B678-2A00A4C74168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data de Atualização" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="233">
-  <si>
-    <t>Data da última atualização: 17/12/21</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="234">
+  <si>
+    <t>Data da última atualização: 01/01/22</t>
   </si>
   <si>
     <t>Porcentagem:</t>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t>Decisões monocráticas</t>
+  </si>
+  <si>
+    <t>MIN. ANDRÉ MENDONÇA</t>
   </si>
   <si>
     <t>Ministros</t>
@@ -3076,19 +3079,19 @@
     <row r="3" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38"/>
       <c r="B3" s="6">
-        <v>26082</v>
+        <v>26127</v>
       </c>
       <c r="C3" s="6">
-        <v>51320</v>
+        <v>51444</v>
       </c>
       <c r="D3" s="12">
-        <v>77402</v>
+        <v>77571</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>3</v>
@@ -3105,13 +3108,13 @@
         <v>57</v>
       </c>
       <c r="B6" s="6">
-        <v>1272</v>
+        <v>1274</v>
       </c>
       <c r="C6" s="6">
-        <v>36312</v>
+        <v>36422</v>
       </c>
       <c r="D6" s="12">
-        <v>37584</v>
+        <v>37696</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3171,10 +3174,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="6">
-        <v>9632</v>
+        <v>10301</v>
       </c>
       <c r="D3" s="7">
-        <v>0.419877942458588</v>
+        <v>0.42774686487833202</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3185,10 +3188,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="8">
-        <v>13308</v>
+        <v>13781</v>
       </c>
       <c r="D4" s="9">
-        <v>0.580122057541412</v>
+        <v>0.57225313512166798</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3197,7 +3200,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="12">
-        <v>22940</v>
+        <v>24082</v>
       </c>
       <c r="D5" s="13">
         <v>1</v>
@@ -3218,10 +3221,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="6">
-        <v>22554</v>
+        <v>23268</v>
       </c>
       <c r="D8" s="7">
-        <v>0.29617470551929698</v>
+        <v>0.30042996036101199</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3232,10 +3235,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="8">
-        <v>53597</v>
+        <v>54181</v>
       </c>
       <c r="D9" s="9">
-        <v>0.70382529448070297</v>
+        <v>0.69957003963898801</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3244,7 +3247,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="12">
-        <v>76151</v>
+        <v>77449</v>
       </c>
       <c r="D10" s="13">
         <v>1</v>
@@ -3265,10 +3268,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="16">
-        <v>871</v>
+        <v>907</v>
       </c>
       <c r="D13" s="9">
-        <v>1.8196252115236001E-2</v>
+        <v>1.88498867344182E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -3279,10 +3282,10 @@
         <v>4</v>
       </c>
       <c r="C14" s="17">
-        <v>46996</v>
+        <v>47210</v>
       </c>
       <c r="D14" s="9">
-        <v>0.98180374788476399</v>
+        <v>0.98115011326558199</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3291,7 +3294,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="12">
-        <v>47867</v>
+        <v>48117</v>
       </c>
       <c r="D15" s="13">
         <v>1</v>
@@ -3316,19 +3319,19 @@
         <v>3</v>
       </c>
       <c r="C18" s="16">
-        <v>21482</v>
+        <v>22202</v>
       </c>
       <c r="D18" s="9">
-        <v>0.66361867103271399</v>
+        <v>0.66942049086413802</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="16">
-        <v>32371</v>
+        <v>33166</v>
       </c>
       <c r="H18" s="9">
-        <v>0.40343727410952401</v>
+        <v>0.40803119963584</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -3339,19 +3342,19 @@
         <v>4</v>
       </c>
       <c r="C19" s="17">
-        <v>10889</v>
+        <v>10964</v>
       </c>
       <c r="D19" s="9">
-        <v>0.33638132896728601</v>
+        <v>0.33057950913586198</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="17">
-        <v>47867</v>
+        <v>48117</v>
       </c>
       <c r="H19" s="9">
-        <v>0.59656272589047599</v>
+        <v>0.59196880036416</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3360,14 +3363,14 @@
         <v>5</v>
       </c>
       <c r="C20" s="12">
-        <v>32371</v>
+        <v>33166</v>
       </c>
       <c r="D20" s="13">
         <v>1</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="12">
-        <v>80238</v>
+        <v>81283</v>
       </c>
       <c r="H20" s="13">
         <v>1</v>
@@ -3390,10 +3393,10 @@
         <v>12</v>
       </c>
       <c r="C23" s="16">
-        <v>15061</v>
+        <v>15417</v>
       </c>
       <c r="D23" s="9">
-        <v>0.156117837299942</v>
+        <v>0.156999124218416</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -3404,10 +3407,10 @@
         <v>13</v>
       </c>
       <c r="C24" s="17">
-        <v>81410</v>
+        <v>82780</v>
       </c>
       <c r="D24" s="9">
-        <v>0.843871796998093</v>
+        <v>0.84299069227479195</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -3421,7 +3424,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="9">
-        <v>1.03657019653371E-5</v>
+        <v>1.0183506792399E-5</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3430,7 +3433,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="12">
-        <v>96472</v>
+        <v>98198</v>
       </c>
       <c r="D26" s="13">
         <v>1</v>
@@ -3453,10 +3456,10 @@
         <v>3</v>
       </c>
       <c r="C29" s="16">
-        <v>8599</v>
+        <v>8752</v>
       </c>
       <c r="D29" s="9">
-        <v>0.46953150595173099</v>
+        <v>0.47165337357189102</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2">
@@ -3467,10 +3470,10 @@
         <v>4</v>
       </c>
       <c r="C30" s="17">
-        <v>9715</v>
+        <v>9804</v>
       </c>
       <c r="D30" s="9">
-        <v>0.53046849404826901</v>
+        <v>0.52834662642810903</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3479,7 +3482,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="12">
-        <v>18314</v>
+        <v>18556</v>
       </c>
       <c r="D31" s="13">
         <v>1</v>
@@ -3500,10 +3503,10 @@
         <v>3</v>
       </c>
       <c r="C34" s="6">
-        <v>26082</v>
+        <v>26127</v>
       </c>
       <c r="D34" s="9">
-        <v>0.33696803700162797</v>
+        <v>0.33681401554704699</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3514,10 +3517,10 @@
         <v>4</v>
       </c>
       <c r="C35" s="8">
-        <v>51320</v>
+        <v>51444</v>
       </c>
       <c r="D35" s="9">
-        <v>0.66303196299837197</v>
+        <v>0.66318598445295296</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3526,7 +3529,7 @@
         <v>5</v>
       </c>
       <c r="C36" s="12">
-        <v>77402</v>
+        <v>77571</v>
       </c>
       <c r="D36" s="13">
         <v>1</v>
@@ -3594,24 +3597,24 @@
       </c>
       <c r="B3" s="41"/>
       <c r="C3" s="45">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="D3" s="45"/>
       <c r="E3" s="6">
-        <v>876</v>
+        <v>871</v>
       </c>
       <c r="F3" s="12">
-        <v>2096</v>
+        <v>2089</v>
       </c>
       <c r="I3" s="41" t="s">
         <v>24</v>
       </c>
       <c r="J3" s="41"/>
       <c r="K3" s="6">
-        <v>22871</v>
+        <v>24017</v>
       </c>
       <c r="L3" s="23">
-        <v>0.99699215344376602</v>
+        <v>0.99730088863051203</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3620,24 +3623,24 @@
       </c>
       <c r="B4" s="41"/>
       <c r="C4" s="48">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D4" s="48"/>
       <c r="E4" s="8">
-        <v>685</v>
+        <v>693</v>
       </c>
       <c r="F4" s="12">
-        <v>1611</v>
+        <v>1618</v>
       </c>
       <c r="I4" s="41" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="41"/>
       <c r="K4" s="8">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="L4" s="24">
-        <v>3.0078465562336501E-3</v>
+        <v>2.69911136948758E-3</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3646,21 +3649,21 @@
       </c>
       <c r="B5" s="41"/>
       <c r="C5" s="45">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D5" s="45"/>
       <c r="E5" s="6">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="F5" s="12">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="I5" s="43" t="s">
         <v>5</v>
       </c>
       <c r="J5" s="43"/>
       <c r="K5" s="12">
-        <v>22940</v>
+        <v>24082</v>
       </c>
       <c r="L5" s="13">
         <v>1</v>
@@ -3672,14 +3675,14 @@
       </c>
       <c r="B6" s="41"/>
       <c r="C6" s="48">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="D6" s="48"/>
       <c r="E6" s="8">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="F6" s="12">
-        <v>1676</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3688,14 +3691,14 @@
       </c>
       <c r="B7" s="41"/>
       <c r="C7" s="45">
-        <v>5800</v>
+        <v>6477</v>
       </c>
       <c r="D7" s="45"/>
       <c r="E7" s="6">
-        <v>10952</v>
+        <v>11416</v>
       </c>
       <c r="F7" s="12">
-        <v>16752</v>
+        <v>17893</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3704,14 +3707,14 @@
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="46">
-        <v>9632</v>
+        <v>10301</v>
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="12">
-        <v>13308</v>
+        <v>13781</v>
       </c>
       <c r="F8" s="12">
-        <v>22940</v>
+        <v>24082</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3734,11 +3737,11 @@
       </c>
       <c r="B11" s="41"/>
       <c r="C11" s="45">
-        <v>9309</v>
+        <v>9606</v>
       </c>
       <c r="D11" s="45"/>
       <c r="E11" s="23">
-        <v>0.40579773321708801</v>
+        <v>0.39888713561996503</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3747,11 +3750,11 @@
       </c>
       <c r="B12" s="41"/>
       <c r="C12" s="48">
-        <v>2916</v>
+        <v>3329</v>
       </c>
       <c r="D12" s="48"/>
       <c r="E12" s="24">
-        <v>0.127114210985179</v>
+        <v>0.138236026908064</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3760,11 +3763,11 @@
       </c>
       <c r="B13" s="41"/>
       <c r="C13" s="45">
-        <v>2614</v>
+        <v>2689</v>
       </c>
       <c r="D13" s="45"/>
       <c r="E13" s="23">
-        <v>0.113949433304272</v>
+        <v>0.111660161116186</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3773,11 +3776,11 @@
       </c>
       <c r="B14" s="41"/>
       <c r="C14" s="48">
-        <v>2097</v>
+        <v>2137</v>
       </c>
       <c r="D14" s="48"/>
       <c r="E14" s="24">
-        <v>9.1412380122057602E-2</v>
+        <v>8.8738476870691793E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3786,11 +3789,11 @@
       </c>
       <c r="B15" s="41"/>
       <c r="C15" s="45">
-        <v>1758</v>
+        <v>1899</v>
       </c>
       <c r="D15" s="45"/>
       <c r="E15" s="23">
-        <v>7.6634699215344396E-2</v>
+        <v>7.88555767793373E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3799,11 +3802,11 @@
       </c>
       <c r="B16" s="41"/>
       <c r="C16" s="48">
-        <v>1172</v>
+        <v>1236</v>
       </c>
       <c r="D16" s="48"/>
       <c r="E16" s="24">
-        <v>5.1089799476896298E-2</v>
+        <v>5.1324640810563898E-2</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3812,11 +3815,11 @@
       </c>
       <c r="B17" s="41"/>
       <c r="C17" s="45">
-        <v>942</v>
+        <v>979</v>
       </c>
       <c r="D17" s="45"/>
       <c r="E17" s="23">
-        <v>4.1063644289450703E-2</v>
+        <v>4.0652769703513003E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -3825,11 +3828,11 @@
       </c>
       <c r="B18" s="41"/>
       <c r="C18" s="48">
-        <v>666</v>
+        <v>707</v>
       </c>
       <c r="D18" s="48"/>
       <c r="E18" s="24">
-        <v>2.9032258064516099E-2</v>
+        <v>2.9358026741964999E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="1" customFormat="1" ht="9.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -3838,11 +3841,11 @@
       </c>
       <c r="B19" s="41"/>
       <c r="C19" s="45">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="D19" s="45"/>
       <c r="E19" s="51">
-        <v>1.1769834350479499E-2</v>
+        <v>1.1377792542147699E-2</v>
       </c>
       <c r="F19" s="53"/>
       <c r="G19" s="53"/>
@@ -3860,7 +3863,7 @@
       </c>
       <c r="G20" s="41"/>
       <c r="H20" s="45">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I20" s="45"/>
     </row>
@@ -3870,11 +3873,11 @@
       </c>
       <c r="B21" s="41"/>
       <c r="C21" s="48">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="D21" s="48"/>
       <c r="E21" s="52">
-        <v>1.0287707061900599E-2</v>
+        <v>1.0173573623453201E-2</v>
       </c>
       <c r="F21" s="41"/>
       <c r="G21" s="41"/>
@@ -3894,11 +3897,11 @@
       </c>
       <c r="B23" s="41"/>
       <c r="C23" s="45">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="D23" s="45"/>
       <c r="E23" s="23">
-        <v>9.8081952920662605E-3</v>
+        <v>9.5507017689560707E-3</v>
       </c>
       <c r="F23" s="40" t="s">
         <v>54</v>
@@ -3917,7 +3920,7 @@
       </c>
       <c r="D24" s="48"/>
       <c r="E24" s="52">
-        <v>8.1517000871839593E-3</v>
+        <v>7.7651357860642799E-3</v>
       </c>
       <c r="F24" s="40"/>
       <c r="G24" s="40"/>
@@ -3948,11 +3951,11 @@
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="45">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="51">
-        <v>7.4978204010462098E-3</v>
+        <v>7.2253135121667601E-3</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="1" customFormat="1" ht="3.2" customHeight="1" x14ac:dyDescent="0.2">
@@ -3974,11 +3977,11 @@
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="48">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D29" s="48"/>
       <c r="E29" s="24">
-        <v>5.2310374891020098E-3</v>
+        <v>5.0660244165766999E-3</v>
       </c>
       <c r="F29" s="40"/>
       <c r="G29" s="40"/>
@@ -3991,11 +3994,11 @@
       </c>
       <c r="B30" s="41"/>
       <c r="C30" s="45">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="51">
-        <v>2.7898866608544E-3</v>
+        <v>2.69911136948758E-3</v>
       </c>
       <c r="F30" s="41"/>
       <c r="G30" s="41"/>
@@ -4015,11 +4018,11 @@
       </c>
       <c r="B32" s="41"/>
       <c r="C32" s="48">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D32" s="48"/>
       <c r="E32" s="52">
-        <v>1.9180470793373999E-3</v>
+        <v>1.9516651440910199E-3</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="1" customFormat="1" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4041,11 +4044,11 @@
       </c>
       <c r="B34" s="41"/>
       <c r="C34" s="45">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D34" s="45"/>
       <c r="E34" s="23">
-        <v>1.2205754141237999E-3</v>
+        <v>1.2042189186944601E-3</v>
       </c>
       <c r="F34" s="40"/>
       <c r="G34" s="40"/>
@@ -4058,18 +4061,18 @@
       </c>
       <c r="B35" s="41"/>
       <c r="C35" s="48">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D35" s="48"/>
       <c r="E35" s="24">
-        <v>1.1333914559721E-3</v>
+        <v>1.1211693380948401E-3</v>
       </c>
       <c r="F35" s="41" t="s">
         <v>57</v>
       </c>
       <c r="G35" s="41"/>
       <c r="H35" s="45">
-        <v>5246</v>
+        <v>5316</v>
       </c>
       <c r="I35" s="45"/>
     </row>
@@ -4079,18 +4082,18 @@
       </c>
       <c r="B36" s="41"/>
       <c r="C36" s="45">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D36" s="45"/>
       <c r="E36" s="23">
-        <v>1.0897994768962499E-3</v>
+        <v>1.0796445477950301E-3</v>
       </c>
       <c r="F36" s="43" t="s">
         <v>5</v>
       </c>
       <c r="G36" s="43"/>
       <c r="H36" s="46">
-        <v>5246</v>
+        <v>5316</v>
       </c>
       <c r="I36" s="46"/>
     </row>
@@ -4100,11 +4103,11 @@
       </c>
       <c r="B37" s="41"/>
       <c r="C37" s="48">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D37" s="48"/>
       <c r="E37" s="24">
-        <v>1.0462074978204001E-3</v>
+        <v>1.0796445477950301E-3</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4113,22 +4116,22 @@
       </c>
       <c r="B38" s="41"/>
       <c r="C38" s="45">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D38" s="45"/>
       <c r="E38" s="23">
-        <v>6.53879686137751E-4</v>
+        <v>7.4744622539656201E-4</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="41"/>
       <c r="B39" s="41"/>
       <c r="C39" s="48">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D39" s="48"/>
       <c r="E39" s="24">
-        <v>5.6669572798605098E-4</v>
+        <v>4.9829748359770797E-4</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4137,11 +4140,11 @@
       </c>
       <c r="B40" s="41"/>
       <c r="C40" s="45">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D40" s="45"/>
       <c r="E40" s="23">
-        <v>4.3591979075850002E-4</v>
+        <v>4.56772693297899E-4</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4154,7 +4157,7 @@
       </c>
       <c r="D41" s="48"/>
       <c r="E41" s="24">
-        <v>1.3077593722755001E-4</v>
+        <v>1.2457437089942699E-4</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4167,7 +4170,7 @@
       </c>
       <c r="D42" s="45"/>
       <c r="E42" s="23">
-        <v>1.3077593722755001E-4</v>
+        <v>1.2457437089942699E-4</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4180,7 +4183,7 @@
       </c>
       <c r="D43" s="48"/>
       <c r="E43" s="24">
-        <v>4.3591979075849999E-5</v>
+        <v>4.1524790299808998E-5</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4198,7 +4201,7 @@
       </c>
       <c r="B45" s="43"/>
       <c r="C45" s="46">
-        <v>22940</v>
+        <v>24082</v>
       </c>
       <c r="D45" s="46"/>
       <c r="E45" s="26"/>
@@ -4215,7 +4218,7 @@
         <v>57</v>
       </c>
       <c r="B47" s="45">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C47" s="45"/>
     </row>
@@ -4224,7 +4227,7 @@
         <v>5</v>
       </c>
       <c r="B48" s="46">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C48" s="46"/>
     </row>
@@ -4378,7 +4381,7 @@
         <v>59</v>
       </c>
       <c r="B3" s="45">
-        <v>53597</v>
+        <v>54181</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
@@ -4394,7 +4397,7 @@
         <v>60</v>
       </c>
       <c r="B5" s="48">
-        <v>559</v>
+        <v>572</v>
       </c>
       <c r="I5" s="40"/>
       <c r="J5" s="44"/>
@@ -4406,7 +4409,7 @@
         <v>3</v>
       </c>
       <c r="J6" s="45">
-        <v>22554</v>
+        <v>23268</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4414,7 +4417,7 @@
         <v>61</v>
       </c>
       <c r="B7" s="45">
-        <v>14245</v>
+        <v>14754</v>
       </c>
       <c r="I7" s="41"/>
       <c r="J7" s="45"/>
@@ -4426,7 +4429,7 @@
         <v>4</v>
       </c>
       <c r="J8" s="48">
-        <v>53597</v>
+        <v>54181</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4434,7 +4437,7 @@
         <v>62</v>
       </c>
       <c r="B9" s="48">
-        <v>7750</v>
+        <v>7942</v>
       </c>
       <c r="I9" s="41"/>
       <c r="J9" s="48"/>
@@ -4446,7 +4449,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="46">
-        <v>76151</v>
+        <v>77449</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4454,7 +4457,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="46">
-        <v>76151</v>
+        <v>77449</v>
       </c>
       <c r="I11" s="43"/>
       <c r="J11" s="46"/>
@@ -4483,13 +4486,13 @@
         <v>65</v>
       </c>
       <c r="B15" s="6">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>60</v>
       </c>
       <c r="G15" s="6">
-        <v>559</v>
+        <v>572</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4497,13 +4500,13 @@
         <v>66</v>
       </c>
       <c r="B16" s="8">
-        <v>42358</v>
+        <v>42812</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>61</v>
       </c>
       <c r="G16" s="8">
-        <v>14245</v>
+        <v>14754</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4511,13 +4514,13 @@
         <v>67</v>
       </c>
       <c r="B17" s="6">
-        <v>11127</v>
+        <v>11255</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>62</v>
       </c>
       <c r="G17" s="6">
-        <v>7750</v>
+        <v>7942</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4525,13 +4528,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="12">
-        <v>53597</v>
+        <v>54181</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G18" s="12">
-        <v>22554</v>
+        <v>23268</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4552,10 +4555,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="6">
-        <v>32371</v>
+        <v>33166</v>
       </c>
       <c r="C21" s="51">
-        <v>0.40343727410952401</v>
+        <v>0.40803119963584</v>
       </c>
       <c r="D21" s="51"/>
     </row>
@@ -4564,10 +4567,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="8">
-        <v>47867</v>
+        <v>48117</v>
       </c>
       <c r="C22" s="52">
-        <v>0.59656272589047599</v>
+        <v>0.59196880036416</v>
       </c>
       <c r="D22" s="52"/>
     </row>
@@ -4576,7 +4579,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="12">
-        <v>80238</v>
+        <v>81283</v>
       </c>
       <c r="C23" s="54">
         <v>1</v>
@@ -4601,10 +4604,10 @@
         <v>8</v>
       </c>
       <c r="B26" s="6">
-        <v>10889</v>
+        <v>10964</v>
       </c>
       <c r="C26" s="51">
-        <v>0.18811436468860701</v>
+        <v>0.18846907553202499</v>
       </c>
       <c r="D26" s="51"/>
     </row>
@@ -4613,10 +4616,10 @@
         <v>9</v>
       </c>
       <c r="B27" s="8">
-        <v>46996</v>
+        <v>47210</v>
       </c>
       <c r="C27" s="52">
-        <v>0.81188563531139302</v>
+        <v>0.81153092446797503</v>
       </c>
       <c r="D27" s="52"/>
     </row>
@@ -4625,7 +4628,7 @@
         <v>5</v>
       </c>
       <c r="B28" s="12">
-        <v>57885</v>
+        <v>58174</v>
       </c>
       <c r="C28" s="54">
         <v>1</v>
@@ -4646,7 +4649,7 @@
         <v>65</v>
       </c>
       <c r="B31" s="6">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4654,7 +4657,7 @@
         <v>66</v>
       </c>
       <c r="B32" s="8">
-        <v>6779</v>
+        <v>6826</v>
       </c>
     </row>
     <row r="33" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4662,7 +4665,7 @@
         <v>67</v>
       </c>
       <c r="B33" s="6">
-        <v>4094</v>
+        <v>4120</v>
       </c>
     </row>
     <row r="34" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4670,7 +4673,7 @@
         <v>5</v>
       </c>
       <c r="B34" s="12">
-        <v>10889</v>
+        <v>10964</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="1" customFormat="1" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4695,7 +4698,7 @@
         <v>66</v>
       </c>
       <c r="B38" s="8">
-        <v>39398</v>
+        <v>39572</v>
       </c>
     </row>
     <row r="39" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4703,7 +4706,7 @@
         <v>67</v>
       </c>
       <c r="B39" s="6">
-        <v>7506</v>
+        <v>7546</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4711,7 +4714,7 @@
         <v>5</v>
       </c>
       <c r="B40" s="12">
-        <v>46996</v>
+        <v>47210</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4746,7 +4749,7 @@
         <v>2</v>
       </c>
       <c r="N45" s="8">
-        <v>5930</v>
+        <v>5929</v>
       </c>
     </row>
     <row r="46" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4768,7 +4771,7 @@
         <v>4</v>
       </c>
       <c r="N47" s="8">
-        <v>6813</v>
+        <v>6812</v>
       </c>
     </row>
     <row r="48" spans="1:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4812,7 +4815,7 @@
         <v>8</v>
       </c>
       <c r="N51" s="8">
-        <v>6131</v>
+        <v>6130</v>
       </c>
     </row>
     <row r="52" spans="12:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4823,7 +4826,7 @@
         <v>9</v>
       </c>
       <c r="N52" s="27">
-        <v>7030</v>
+        <v>7029</v>
       </c>
     </row>
     <row r="53" spans="12:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4834,7 +4837,7 @@
         <v>10</v>
       </c>
       <c r="N53" s="8">
-        <v>5485</v>
+        <v>5483</v>
       </c>
     </row>
     <row r="54" spans="12:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4845,7 +4848,7 @@
         <v>11</v>
       </c>
       <c r="N54" s="27">
-        <v>7639</v>
+        <v>7637</v>
       </c>
     </row>
     <row r="55" spans="12:14" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -4856,7 +4859,7 @@
         <v>12</v>
       </c>
       <c r="N55" s="8">
-        <v>4986</v>
+        <v>6292</v>
       </c>
     </row>
     <row r="56" spans="12:14" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4925,7 +4928,7 @@
         <v>60</v>
       </c>
       <c r="B3" s="6">
-        <v>559</v>
+        <v>572</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4933,7 +4936,7 @@
         <v>61</v>
       </c>
       <c r="B4" s="8">
-        <v>14245</v>
+        <v>14754</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4941,7 +4944,7 @@
         <v>62</v>
       </c>
       <c r="B5" s="6">
-        <v>7750</v>
+        <v>7942</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4949,7 +4952,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="12">
-        <v>22554</v>
+        <v>23268</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1" ht="22.35" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4980,7 +4983,7 @@
         <v>75</v>
       </c>
       <c r="C10" s="8">
-        <v>399</v>
+        <v>405</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5002,7 +5005,7 @@
         <v>77</v>
       </c>
       <c r="C12" s="8">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5011,7 +5014,7 @@
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="12">
-        <v>559</v>
+        <v>572</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5053,7 +5056,7 @@
         <v>80</v>
       </c>
       <c r="C18" s="6">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5064,7 +5067,7 @@
         <v>81</v>
       </c>
       <c r="C19" s="8">
-        <v>12213</v>
+        <v>12702</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5075,7 +5078,7 @@
         <v>82</v>
       </c>
       <c r="C20" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5086,7 +5089,7 @@
         <v>83</v>
       </c>
       <c r="C21" s="8">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5108,7 +5111,7 @@
         <v>85</v>
       </c>
       <c r="C23" s="8">
-        <v>1906</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5128,7 +5131,7 @@
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="12">
-        <v>14245</v>
+        <v>14754</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5148,7 +5151,7 @@
         <v>87</v>
       </c>
       <c r="C28" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5159,7 +5162,7 @@
         <v>88</v>
       </c>
       <c r="C29" s="8">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5192,7 +5195,7 @@
         <v>91</v>
       </c>
       <c r="C32" s="6">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5214,7 +5217,7 @@
         <v>93</v>
       </c>
       <c r="C34" s="6">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5258,7 +5261,7 @@
         <v>97</v>
       </c>
       <c r="C38" s="6">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5269,7 +5272,7 @@
         <v>98</v>
       </c>
       <c r="C39" s="8">
-        <v>594</v>
+        <v>611</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5280,7 +5283,7 @@
         <v>99</v>
       </c>
       <c r="C40" s="6">
-        <v>571</v>
+        <v>588</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5291,7 +5294,7 @@
         <v>100</v>
       </c>
       <c r="C41" s="8">
-        <v>5746</v>
+        <v>5882</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5324,7 +5327,7 @@
         <v>103</v>
       </c>
       <c r="C44" s="6">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5346,7 +5349,7 @@
         <v>105</v>
       </c>
       <c r="C46" s="6">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5357,7 +5360,7 @@
         <v>106</v>
       </c>
       <c r="C47" s="8">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:3" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5379,7 +5382,7 @@
         <v>108</v>
       </c>
       <c r="C49" s="8">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5399,7 +5402,7 @@
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="12">
-        <v>7750</v>
+        <v>7942</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="1" customFormat="1" ht="178.15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5433,7 +5436,7 @@
         <v>2</v>
       </c>
       <c r="G55" s="8">
-        <v>5930</v>
+        <v>5929</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5455,7 +5458,7 @@
         <v>4</v>
       </c>
       <c r="G57" s="8">
-        <v>6813</v>
+        <v>6812</v>
       </c>
     </row>
     <row r="58" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5499,7 +5502,7 @@
         <v>8</v>
       </c>
       <c r="G61" s="8">
-        <v>6131</v>
+        <v>6130</v>
       </c>
     </row>
     <row r="62" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5510,7 +5513,7 @@
         <v>9</v>
       </c>
       <c r="G62" s="27">
-        <v>7030</v>
+        <v>7029</v>
       </c>
     </row>
     <row r="63" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5521,7 +5524,7 @@
         <v>10</v>
       </c>
       <c r="G63" s="8">
-        <v>5485</v>
+        <v>5483</v>
       </c>
     </row>
     <row r="64" spans="1:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5532,7 +5535,7 @@
         <v>11</v>
       </c>
       <c r="G64" s="27">
-        <v>7639</v>
+        <v>7637</v>
       </c>
     </row>
     <row r="65" spans="5:7" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5543,7 +5546,7 @@
         <v>12</v>
       </c>
       <c r="G65" s="8">
-        <v>4986</v>
+        <v>6292</v>
       </c>
     </row>
     <row r="66" spans="5:7" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5592,14 +5595,14 @@
         <v>111</v>
       </c>
       <c r="B3" s="6">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C3" s="6">
-        <v>2723</v>
+        <v>2788</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="12">
-        <v>2765</v>
+        <v>2833</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5610,11 +5613,11 @@
         <v>14</v>
       </c>
       <c r="C4" s="8">
-        <v>3578</v>
+        <v>3661</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="12">
-        <v>3592</v>
+        <v>3675</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5622,16 +5625,16 @@
         <v>113</v>
       </c>
       <c r="B5" s="6">
-        <v>1591</v>
+        <v>1614</v>
       </c>
       <c r="C5" s="6">
-        <v>72831</v>
+        <v>74017</v>
       </c>
       <c r="D5" s="6">
         <v>1</v>
       </c>
       <c r="E5" s="12">
-        <v>74423</v>
+        <v>75632</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5639,14 +5642,14 @@
         <v>114</v>
       </c>
       <c r="B6" s="8">
-        <v>13283</v>
+        <v>13608</v>
       </c>
       <c r="C6" s="8">
-        <v>1698</v>
+        <v>1721</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="12">
-        <v>14981</v>
+        <v>15329</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5654,12 +5657,12 @@
         <v>115</v>
       </c>
       <c r="B7" s="6">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="12">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5668,11 +5671,11 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="12">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5681,11 +5684,11 @@
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
-        <v>475</v>
+        <v>484</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="12">
-        <v>475</v>
+        <v>484</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5693,16 +5696,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="12">
-        <v>15061</v>
+        <v>15417</v>
       </c>
       <c r="C10" s="12">
-        <v>81410</v>
+        <v>82780</v>
       </c>
       <c r="D10" s="12">
         <v>1</v>
       </c>
       <c r="E10" s="12">
-        <v>96472</v>
+        <v>98198</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5719,7 +5722,7 @@
         <v>119</v>
       </c>
       <c r="B13" s="6">
-        <v>40811</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5727,7 +5730,7 @@
         <v>120</v>
       </c>
       <c r="B14" s="8">
-        <v>15</v>
+        <v>41854</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5735,21 +5738,28 @@
         <v>121</v>
       </c>
       <c r="B15" s="6">
-        <v>40584</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="8">
+        <v>40908</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="12">
-        <v>81410</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="1" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B17" s="12">
+        <v>82780</v>
+      </c>
+    </row>
     <row r="18" spans="1:2" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>12</v>
@@ -5757,18 +5767,18 @@
     </row>
     <row r="19" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B19" s="6">
-        <v>4897</v>
+        <v>5073</v>
       </c>
     </row>
     <row r="20" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B20" s="8">
-        <v>10164</v>
+        <v>10344</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5776,13 +5786,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="12">
-        <v>15061</v>
+        <v>15417</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="1" customFormat="1" ht="12.2" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:2" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>12</v>
@@ -5790,34 +5800,34 @@
     </row>
     <row r="24" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B24" s="6">
-        <v>5794</v>
+        <v>5899</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B25" s="8">
-        <v>4370</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="26" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B26" s="6">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B27" s="8">
-        <v>4814</v>
+        <v>4987</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5825,13 +5835,13 @@
         <v>5</v>
       </c>
       <c r="B28" s="12">
-        <v>15061</v>
+        <v>15417</v>
       </c>
     </row>
     <row r="29" spans="1:2" s="1" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:2" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>12</v>
@@ -5839,10 +5849,10 @@
     </row>
     <row r="31" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B31" s="6">
-        <v>3767</v>
+        <v>3904</v>
       </c>
     </row>
     <row r="32" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5850,7 +5860,7 @@
         <v>60</v>
       </c>
       <c r="B32" s="8">
-        <v>544</v>
+        <v>562</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5866,7 +5876,7 @@
         <v>62</v>
       </c>
       <c r="B34" s="8">
-        <v>495</v>
+        <v>516</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -5880,7 +5890,7 @@
         <v>5</v>
       </c>
       <c r="B36" s="12">
-        <v>4897</v>
+        <v>5073</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="1" customFormat="1" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5919,34 +5929,34 @@
     </row>
     <row r="39" spans="1:12" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="L39" s="22" t="s">
         <v>5</v>
@@ -5954,7 +5964,7 @@
     </row>
     <row r="40" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B40" s="6">
         <v>406</v>
@@ -5984,15 +5994,15 @@
         <v>630</v>
       </c>
       <c r="K40" s="6">
-        <v>286</v>
+        <v>391</v>
       </c>
       <c r="L40" s="12">
-        <v>5486</v>
+        <v>5591</v>
       </c>
     </row>
     <row r="41" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B41" s="8">
         <v>457</v>
@@ -6022,15 +6032,15 @@
         <v>357</v>
       </c>
       <c r="K41" s="8">
-        <v>200</v>
+        <v>275</v>
       </c>
       <c r="L41" s="12">
-        <v>4271</v>
+        <v>4346</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B42" s="6">
         <v>428</v>
@@ -6060,10 +6070,10 @@
         <v>441</v>
       </c>
       <c r="K42" s="6">
-        <v>176</v>
+        <v>347</v>
       </c>
       <c r="L42" s="12">
-        <v>4651</v>
+        <v>4822</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6098,10 +6108,10 @@
         <v>1428</v>
       </c>
       <c r="K43" s="12">
-        <v>662</v>
+        <v>1013</v>
       </c>
       <c r="L43" s="12">
-        <v>14408</v>
+        <v>14759</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="1" customFormat="1" ht="45.4" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6118,7 +6128,7 @@
     </row>
     <row r="46" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B46" s="6">
         <v>24</v>
@@ -6132,142 +6142,142 @@
     </row>
     <row r="47" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B47" s="8">
         <v>79</v>
       </c>
       <c r="C47" s="8">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D47" s="12">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:12" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B48" s="6">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C48" s="6">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D48" s="12">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B49" s="8">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C49" s="8">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D49" s="12">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B50" s="6">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C50" s="6">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D50" s="12">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B51" s="8">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C51" s="8">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D51" s="12">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B52" s="6">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C52" s="6">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D52" s="12">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B53" s="8">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C53" s="8">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D53" s="12">
-        <v>550</v>
+        <v>557</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B54" s="6">
-        <v>516</v>
+        <v>525</v>
       </c>
       <c r="C54" s="6">
-        <v>370</v>
+        <v>378</v>
       </c>
       <c r="D54" s="12">
-        <v>886</v>
+        <v>903</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B55" s="8">
-        <v>1317</v>
+        <v>1330</v>
       </c>
       <c r="C55" s="8">
-        <v>849</v>
+        <v>866</v>
       </c>
       <c r="D55" s="12">
-        <v>2166</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B56" s="6">
-        <v>7013</v>
+        <v>7043</v>
       </c>
       <c r="C56" s="6">
-        <v>6609</v>
+        <v>6642</v>
       </c>
       <c r="D56" s="12">
-        <v>13622</v>
+        <v>13685</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6275,41 +6285,41 @@
         <v>22</v>
       </c>
       <c r="B57" s="8">
-        <v>26979</v>
+        <v>27818</v>
       </c>
       <c r="C57" s="8">
-        <v>50248</v>
+        <v>50988</v>
       </c>
       <c r="D57" s="12">
-        <v>77227</v>
+        <v>78806</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B58" s="6">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C58" s="6">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D58" s="12">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B59" s="8">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C59" s="8">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D59" s="12">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6317,30 +6327,30 @@
         <v>5</v>
       </c>
       <c r="B60" s="12">
-        <v>37364</v>
+        <v>38276</v>
       </c>
       <c r="C60" s="12">
-        <v>59108</v>
+        <v>59922</v>
       </c>
       <c r="D60" s="12">
-        <v>96472</v>
+        <v>98198</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C61" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H61" s="22" t="s">
         <v>5</v>
@@ -6348,7 +6358,7 @@
     </row>
     <row r="62" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>65</v>
@@ -6370,50 +6380,50 @@
     </row>
     <row r="63" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C63" s="8">
-        <v>936</v>
+        <v>957</v>
       </c>
       <c r="D63" s="8">
-        <v>1094</v>
+        <v>1109</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="8">
         <v>25</v>
       </c>
       <c r="G63" s="8">
-        <v>3263</v>
+        <v>3382</v>
       </c>
       <c r="H63" s="12">
-        <v>5318</v>
+        <v>5473</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C64" s="6">
-        <v>602</v>
+        <v>610</v>
       </c>
       <c r="D64" s="6">
-        <v>573</v>
+        <v>585</v>
       </c>
       <c r="E64" s="6"/>
       <c r="F64" s="6">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G64" s="6">
-        <v>414</v>
+        <v>429</v>
       </c>
       <c r="H64" s="12">
-        <v>1647</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6428,10 +6438,10 @@
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H65" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6446,10 +6456,10 @@
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
       <c r="G66" s="6">
-        <v>434</v>
+        <v>448</v>
       </c>
       <c r="H66" s="12">
-        <v>434</v>
+        <v>448</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6482,10 +6492,10 @@
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
       <c r="G68" s="6">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H68" s="12">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6556,10 +6566,10 @@
         <v>81</v>
       </c>
       <c r="C72" s="6">
-        <v>2175</v>
+        <v>2216</v>
       </c>
       <c r="D72" s="6">
-        <v>1207</v>
+        <v>1223</v>
       </c>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
@@ -6567,7 +6577,7 @@
         <v>62</v>
       </c>
       <c r="H72" s="12">
-        <v>3444</v>
+        <v>3501</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6618,10 +6628,10 @@
         <v>85</v>
       </c>
       <c r="C75" s="8">
-        <v>562</v>
+        <v>570</v>
       </c>
       <c r="D75" s="8">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="E75" s="8">
         <v>1</v>
@@ -6631,7 +6641,7 @@
         <v>5</v>
       </c>
       <c r="H75" s="12">
-        <v>829</v>
+        <v>841</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6686,10 +6696,10 @@
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
       <c r="G78" s="6">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="H78" s="12">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6714,7 +6724,7 @@
         <v>90</v>
       </c>
       <c r="C80" s="6">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D80" s="6">
         <v>13</v>
@@ -6725,7 +6735,7 @@
         <v>8</v>
       </c>
       <c r="H80" s="12">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6758,10 +6768,10 @@
       <c r="E82" s="6"/>
       <c r="F82" s="6"/>
       <c r="G82" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H82" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6840,18 +6850,18 @@
         <v>98</v>
       </c>
       <c r="C87" s="8">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D87" s="8">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E87" s="8"/>
       <c r="F87" s="8"/>
       <c r="G87" s="8">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="H87" s="12">
-        <v>358</v>
+        <v>370</v>
       </c>
     </row>
     <row r="88" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6865,7 +6875,7 @@
         <v>49</v>
       </c>
       <c r="D88" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E88" s="6"/>
       <c r="F88" s="6"/>
@@ -6873,7 +6883,7 @@
         <v>25</v>
       </c>
       <c r="H88" s="12">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="89" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6884,18 +6894,18 @@
         <v>100</v>
       </c>
       <c r="C89" s="8">
-        <v>1135</v>
+        <v>1155</v>
       </c>
       <c r="D89" s="8">
-        <v>1081</v>
+        <v>1107</v>
       </c>
       <c r="E89" s="8"/>
       <c r="F89" s="8"/>
       <c r="G89" s="8">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H89" s="12">
-        <v>2226</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="90" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6955,7 +6965,7 @@
         <v>62</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
@@ -6994,10 +7004,10 @@
       <c r="E95" s="8"/>
       <c r="F95" s="8"/>
       <c r="G95" s="8">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H95" s="12">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="96" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -7048,10 +7058,10 @@
       <c r="E98" s="6"/>
       <c r="F98" s="6"/>
       <c r="G98" s="6">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H98" s="12">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="99" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -7094,36 +7104,36 @@
         <v>5</v>
       </c>
       <c r="C101" s="12">
-        <v>5794</v>
+        <v>5899</v>
       </c>
       <c r="D101" s="12">
-        <v>4370</v>
+        <v>4445</v>
       </c>
       <c r="E101" s="12">
         <v>1</v>
       </c>
       <c r="F101" s="12">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G101" s="12">
-        <v>4814</v>
+        <v>4987</v>
       </c>
       <c r="H101" s="12">
-        <v>15062</v>
+        <v>15418</v>
       </c>
     </row>
     <row r="102" spans="1:8" s="1" customFormat="1" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="103" spans="1:8" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="104" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="31" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B104" s="31" t="s">
         <v>87</v>
@@ -7131,7 +7141,7 @@
     </row>
     <row r="105" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="32" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B105" s="32" t="s">
         <v>88</v>
@@ -7139,7 +7149,7 @@
     </row>
     <row r="106" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="31" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B106" s="31" t="s">
         <v>74</v>
@@ -7147,7 +7157,7 @@
     </row>
     <row r="107" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="32" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B107" s="32" t="s">
         <v>75</v>
@@ -7155,7 +7165,7 @@
     </row>
     <row r="108" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="31" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B108" s="31" t="s">
         <v>76</v>
@@ -7163,7 +7173,7 @@
     </row>
     <row r="109" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="32" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B109" s="32" t="s">
         <v>90</v>
@@ -7171,7 +7181,7 @@
     </row>
     <row r="110" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="31" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B110" s="31" t="s">
         <v>78</v>
@@ -7179,7 +7189,7 @@
     </row>
     <row r="111" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="32" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B111" s="32" t="s">
         <v>91</v>
@@ -7187,7 +7197,7 @@
     </row>
     <row r="112" spans="1:8" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="31" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B112" s="31" t="s">
         <v>65</v>
@@ -7195,7 +7205,7 @@
     </row>
     <row r="113" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="32" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B113" s="32" t="s">
         <v>77</v>
@@ -7203,7 +7213,7 @@
     </row>
     <row r="114" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="31" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B114" s="31" t="s">
         <v>89</v>
@@ -7211,7 +7221,7 @@
     </row>
     <row r="115" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="32" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B115" s="32" t="s">
         <v>92</v>
@@ -7219,7 +7229,7 @@
     </row>
     <row r="116" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="31" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B116" s="31" t="s">
         <v>93</v>
@@ -7227,7 +7237,7 @@
     </row>
     <row r="117" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="32" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B117" s="32" t="s">
         <v>79</v>
@@ -7235,7 +7245,7 @@
     </row>
     <row r="118" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="31" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B118" s="31" t="s">
         <v>80</v>
@@ -7243,7 +7253,7 @@
     </row>
     <row r="119" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="32" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B119" s="32" t="s">
         <v>81</v>
@@ -7251,7 +7261,7 @@
     </row>
     <row r="120" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="31" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B120" s="31" t="s">
         <v>95</v>
@@ -7259,7 +7269,7 @@
     </row>
     <row r="121" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="32" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B121" s="32" t="s">
         <v>82</v>
@@ -7267,7 +7277,7 @@
     </row>
     <row r="122" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="31" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B122" s="31" t="s">
         <v>96</v>
@@ -7275,7 +7285,7 @@
     </row>
     <row r="123" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="32" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B123" s="32" t="s">
         <v>97</v>
@@ -7283,7 +7293,7 @@
     </row>
     <row r="124" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="31" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B124" s="31" t="s">
         <v>98</v>
@@ -7291,7 +7301,7 @@
     </row>
     <row r="125" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="32" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B125" s="32" t="s">
         <v>99</v>
@@ -7299,7 +7309,7 @@
     </row>
     <row r="126" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="31" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B126" s="31" t="s">
         <v>83</v>
@@ -7307,7 +7317,7 @@
     </row>
     <row r="127" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="32" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B127" s="32" t="s">
         <v>100</v>
@@ -7315,7 +7325,7 @@
     </row>
     <row r="128" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="31" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B128" s="31" t="s">
         <v>84</v>
@@ -7323,7 +7333,7 @@
     </row>
     <row r="129" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="32" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B129" s="32" t="s">
         <v>67</v>
@@ -7331,7 +7341,7 @@
     </row>
     <row r="130" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="31" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B130" s="31" t="s">
         <v>66</v>
@@ -7339,7 +7349,7 @@
     </row>
     <row r="131" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="32" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B131" s="32" t="s">
         <v>103</v>
@@ -7347,7 +7357,7 @@
     </row>
     <row r="132" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="31" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B132" s="31" t="s">
         <v>85</v>
@@ -7355,7 +7365,7 @@
     </row>
     <row r="133" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="32" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B133" s="32" t="s">
         <v>101</v>
@@ -7363,7 +7373,7 @@
     </row>
     <row r="134" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="31" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B134" s="31" t="s">
         <v>102</v>
@@ -7371,7 +7381,7 @@
     </row>
     <row r="135" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="32" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B135" s="32" t="s">
         <v>86</v>
@@ -7379,15 +7389,15 @@
     </row>
     <row r="136" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="31" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B136" s="31" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="137" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="32" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B137" s="32" t="s">
         <v>105</v>
@@ -7395,7 +7405,7 @@
     </row>
     <row r="138" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="31" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B138" s="31" t="s">
         <v>106</v>
@@ -7403,7 +7413,7 @@
     </row>
     <row r="139" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="32" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B139" s="32" t="s">
         <v>107</v>
@@ -7411,7 +7421,7 @@
     </row>
     <row r="140" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="31" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B140" s="31" t="s">
         <v>108</v>
@@ -7419,7 +7429,7 @@
     </row>
     <row r="141" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="32" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B141" s="32" t="s">
         <v>104</v>
@@ -7427,7 +7437,7 @@
     </row>
     <row r="142" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="31" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B142" s="31" t="s">
         <v>109</v>
@@ -7465,31 +7475,31 @@
     <row r="1" spans="1:9" s="1" customFormat="1" ht="34.15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -7500,7 +7510,7 @@
         <v>1303852</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D3" s="34">
         <v>44235</v>
@@ -7509,13 +7519,13 @@
         <v>13</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G3" s="31" t="s">
         <v>113</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I3" s="27">
         <v>1</v>
@@ -7529,7 +7539,7 @@
         <v>1307860</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D4" s="36">
         <v>44328</v>
@@ -7538,13 +7548,13 @@
         <v>13</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G4" s="32" t="s">
         <v>113</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I4" s="8">
         <v>1</v>
@@ -7558,7 +7568,7 @@
         <v>1309975</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D5" s="34">
         <v>44393</v>
@@ -7567,13 +7577,13 @@
         <v>13</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>113</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I5" s="27">
         <v>1</v>
@@ -7587,7 +7597,7 @@
         <v>1327899</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D6" s="36">
         <v>44370</v>
@@ -7596,13 +7606,13 @@
         <v>13</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G6" s="32" t="s">
         <v>113</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I6" s="8">
         <v>1</v>
@@ -7616,7 +7626,7 @@
         <v>1332416</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D7" s="34">
         <v>44382</v>
@@ -7625,13 +7635,13 @@
         <v>13</v>
       </c>
       <c r="F7" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>113</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I7" s="27">
         <v>1</v>
@@ -7645,7 +7655,7 @@
         <v>1332495</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D8" s="36">
         <v>44382</v>
@@ -7654,13 +7664,13 @@
         <v>13</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G8" s="32" t="s">
         <v>113</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I8" s="8">
         <v>1</v>
@@ -7674,7 +7684,7 @@
         <v>1333105</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D9" s="34">
         <v>44382</v>
@@ -7683,13 +7693,13 @@
         <v>13</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G9" s="31" t="s">
         <v>113</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I9" s="27">
         <v>1</v>
@@ -7703,7 +7713,7 @@
         <v>1335466</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D10" s="36">
         <v>44390</v>
@@ -7712,13 +7722,13 @@
         <v>13</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G10" s="32" t="s">
         <v>113</v>
       </c>
       <c r="H10" s="32" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I10" s="8">
         <v>1</v>
@@ -7732,7 +7742,7 @@
         <v>1335979</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D11" s="34">
         <v>44393</v>
@@ -7741,13 +7751,13 @@
         <v>13</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G11" s="31" t="s">
         <v>113</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I11" s="27">
         <v>1</v>
@@ -7761,7 +7771,7 @@
         <v>1340930</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D12" s="36">
         <v>44484</v>
@@ -7770,13 +7780,13 @@
         <v>13</v>
       </c>
       <c r="F12" s="32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G12" s="32" t="s">
         <v>113</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I12" s="8">
         <v>1</v>
@@ -7790,7 +7800,7 @@
         <v>1341860</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D13" s="34">
         <v>44484</v>
@@ -7799,13 +7809,13 @@
         <v>13</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G13" s="31" t="s">
         <v>113</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I13" s="27">
         <v>1</v>
@@ -7819,7 +7829,7 @@
         <v>613241</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D14" s="36">
         <v>44322</v>
@@ -7828,13 +7838,13 @@
         <v>13</v>
       </c>
       <c r="F14" s="32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G14" s="32" t="s">
         <v>113</v>
       </c>
       <c r="H14" s="32" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I14" s="8">
         <v>1</v>
@@ -7848,7 +7858,7 @@
         <v>1103878</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D15" s="34">
         <v>44504</v>
@@ -7857,13 +7867,13 @@
         <v>13</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G15" s="31" t="s">
         <v>113</v>
       </c>
       <c r="H15" s="31" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I15" s="27">
         <v>1</v>
@@ -7877,7 +7887,7 @@
         <v>1303212</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D16" s="36">
         <v>44230</v>
@@ -7886,13 +7896,13 @@
         <v>13</v>
       </c>
       <c r="F16" s="32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G16" s="32" t="s">
         <v>113</v>
       </c>
       <c r="H16" s="32" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I16" s="8">
         <v>1</v>
@@ -7906,7 +7916,7 @@
         <v>1323228</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D17" s="34">
         <v>44474</v>
@@ -7915,13 +7925,13 @@
         <v>13</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G17" s="31" t="s">
         <v>113</v>
       </c>
       <c r="H17" s="31" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I17" s="27">
         <v>1</v>
@@ -7983,7 +7993,7 @@
     <row r="1" spans="1:4" s="1" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:4" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -7998,19 +8008,19 @@
     <row r="3" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38"/>
       <c r="B3" s="6">
-        <v>37364</v>
+        <v>38276</v>
       </c>
       <c r="C3" s="6">
-        <v>59108</v>
+        <v>59922</v>
       </c>
       <c r="D3" s="12">
-        <v>96472</v>
+        <v>98198</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>3</v>
@@ -8025,19 +8035,19 @@
     <row r="6" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="38"/>
       <c r="B6" s="6">
-        <v>8599</v>
+        <v>8752</v>
       </c>
       <c r="C6" s="6">
-        <v>9715</v>
+        <v>9804</v>
       </c>
       <c r="D6" s="12">
-        <v>18314</v>
+        <v>18556</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>3</v>
@@ -8052,19 +8062,19 @@
     <row r="9" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="38"/>
       <c r="B9" s="6">
-        <v>1220</v>
+        <v>1271</v>
       </c>
       <c r="C9" s="6">
-        <v>42823</v>
+        <v>43232</v>
       </c>
       <c r="D9" s="12">
-        <v>44043</v>
+        <v>44503</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" ht="46.35" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:4" s="1" customFormat="1" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="39" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>3</v>
@@ -8079,13 +8089,13 @@
     <row r="12" spans="1:4" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="38"/>
       <c r="B12" s="6">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="C12" s="6">
-        <v>5059</v>
+        <v>5101</v>
       </c>
       <c r="D12" s="12">
-        <v>5271</v>
+        <v>5321</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8101,7 +8111,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8113,16 +8125,16 @@
     <row r="1" spans="1:2" s="1" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:2" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B3" s="6">
-        <v>15876</v>
+        <v>16069</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>